<commit_message>
the program is finished
</commit_message>
<xml_diff>
--- a/my_name.xlsx
+++ b/my_name.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,11 +477,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>84062871</v>
+        <v>84067668</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Стажер Python developer (СКИИС)</t>
+          <t>Технический директор / СТО / CIO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -491,33 +491,33 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>МТС</t>
+          <t>Work&amp;Wolf</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/84062871</t>
+          <t>https://hh.ru/vacancy/84067668</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Опыт написания скриптов на PowerShell или Bash/Shell (либо наличие опыта разработки на C#) . Навыки проведение диагностики, анализ логов и...</t>
+          <t>Опыт Solution Architect. Опыт формирования команды R&amp;D. Хорошее знание и применение на практике современных технологических стеков. Постоянный анализ конъюнктуры...</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>600000</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>84046041</v>
+        <v>84115928</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Junior Data Scientist (Специалист по анализу данных)</t>
+          <t>Директор по персоналу</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -527,17 +527,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>АлгоМост</t>
+          <t>НЕД</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/84046041</t>
+          <t>https://hh.ru/vacancy/84115928</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Знание в сфере анализа данных, машинного обучения, статистики (методы, модели, способы их реализации и поддержки).  Python&lt;/highlighttext&gt;, стандартный ML-стэком(numpy...</t>
+          <t>Образование Высшее. Опыт работы Директором по персоналу в крупных торгово-производственных компаниях от 5 лет. Опыт работы с первыми лицами...</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -549,11 +549,11 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>84024689</v>
+        <v>84013893</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Junior Python-разработчик</t>
+          <t>Директор технический</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -563,33 +563,33 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>СОГАЗ</t>
+          <t>Ходынский Парк</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/84024689</t>
+          <t>https://hh.ru/vacancy/84013893</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Уверенное знание  Python&lt;/highlighttext&gt;. Уверенное знание PostgreSQL и умение писать оптимизированные запросы. Опыт работы с Git. Знание принципов работы nginx, gunicorn.</t>
+          <t>Высшее профильное образование (строительное, энергетическое). Опыт работы руководителем службы инженерно-технической эксплуатации, техническим директором на объектах недвижимости, главным инженером не...</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>226000</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>227000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>83618124</v>
+        <v>83722923</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Junior Backend developer (Python)</t>
+          <t>Главный энергетик</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -599,21 +599,21 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Effective Mobile</t>
+          <t>Impar S.R.L.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83618124</t>
+          <t>https://hh.ru/vacancy/83722923</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Знание  python&lt;/highlighttext&gt;. Желание развиваться в сфере backend-разработки. Понимание REST API, базовые знания SQL и NoSQL, умение работать с Git. </t>
+          <t xml:space="preserve">Высшее профильное образование. Успешный опыт работы по специальности не менее 10 лет. V до и свыше 1000в. </t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>226000</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -621,11 +621,11 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>83964034</v>
+        <v>83953222</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Junior Data Scientist</t>
+          <t>Диспетчер</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -635,33 +635,33 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ренессанс cтрахование, Группа</t>
+          <t>ТСК Мосэнерго</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83964034</t>
+          <t>https://hh.ru/vacancy/83953222</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Имеет навыки построения моделей машинного обучения. Владеет математической статистикой, линейной алгеброй. Знает  Python&lt;/highlighttext&gt; (pandas, sklearn, numpy, matplotlib). Владеет SQL. </t>
+          <t xml:space="preserve">Образование не ниже среднего профессионального (теплоэнергетическое, теплотехническое). Опыт работы по специальности не менее 1 года. Знание правил техники безопасности. </t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>59000</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>84020515</v>
+        <v>83198910</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>QA инженер</t>
+          <t>Менеджер по продажам</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -671,21 +671,21 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>НПФ Будущее</t>
+          <t>УЦ Техстандарт</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/84020515</t>
+          <t>https://hh.ru/vacancy/83198910</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Умение работать в системах: Битрикс24, Redmine, TMS Test IT. Базовые знания  Python&lt;/highlighttext&gt;(PEP8). Базовые знания NoSQL (mongo, redis).</t>
+          <t>Среднее специальное или высшее образование. Опыт работы в учебном центре ДПО приветствуется. Грамотная устная и письменная речь, хорошо развитые коммуникативные...</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>59000</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -693,11 +693,11 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>83761018</v>
+        <v>83994538</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Программист Python</t>
+          <t>Заместитель коммерческого директора</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -707,21 +707,21 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>MedMundus</t>
+          <t>САМПЛЕКС</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83761018</t>
+          <t>https://hh.ru/vacancy/83994538</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Опыт использования ORM и понимание принципов построения SQL запросов. - Опыт CI/CD  Python&lt;/highlighttext&gt; приложений. - Опыт разработки продуктов с нуля / с...</t>
+          <t>Коммерсант c большой буквы! Обладание огромной  энергетикой&lt;/highlighttext&gt;, настойчивость, умение добиваться целей и поставленных задач любыми способами, гибкость и аналитический склад...</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>59000</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -729,11 +729,11 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>83689287</v>
+        <v>83830672</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Data Science Intern (LLM)</t>
+          <t>Пеший Курьер</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -743,33 +743,33 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>AIR</t>
+          <t>Поставщик счастья</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83689287</t>
+          <t>https://hh.ru/vacancy/83830672</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Начальные знания в области NLP (обработки естественного языка). Знание английского языка на уровне В1 и выше. Опыт в хакатонах...</t>
+          <t>Нам нужен человек- энергетик&lt;/highlighttext&gt; со знаком "плюс" :). Хорошее знание города. Ответственность, пунктуальность, аккуратность. Приветствуется опыт работы в интернет-магазинах и...</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>84026782</v>
+        <v>84067311</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Junior Data Scientist (NLP)/GPT Prompt инженер/Лингвист)</t>
+          <t>Главный эксперт Управления инвестиционного анализа</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -779,21 +779,21 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Bewise.ai</t>
+          <t>РусГидро</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/84026782</t>
+          <t>https://hh.ru/vacancy/84067311</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Базовые знания о LLM и принципах их работы. Опыт программирования на  Python&lt;/highlighttext&gt; от 1 года (numpy, scipy, pandas). </t>
+          <t xml:space="preserve">Стаж работы по профилю деятельности Управления/Департамента не менее 5 лет. Желателен стаж работы в  энергетике&lt;/highlighttext&gt; или с энергетическими проектами. </t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -801,11 +801,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>84062980</v>
+        <v>83939236</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Программист Python</t>
+          <t>Директор по развитию бизнеса (энергетика)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -815,21 +815,21 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Инжиниринговый Центр Железнодорожного Транспорта</t>
+          <t>SocioTeam Сonsulting</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/84062980</t>
+          <t>https://hh.ru/vacancy/83939236</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Алексеева). Владение языком программирования  Python&lt;/highlighttext&gt; на уровне Junior/Middle. Владение библиотеками Numpy, Scipy, Matplotlib и им подобным. Автоматизация Excel-таблиц. </t>
+          <t>Опыт в привлечении и развитии проектов за рубежом, включая поставки оборудования. Умение налаживать деловые контакты с нуля и успешно развивать...</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -837,11 +837,11 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>83813635</v>
+        <v>83080852</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Python разработчик junior</t>
+          <t>Руководитель направления</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -851,33 +851,33 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>amoCRM</t>
+          <t>Фонд поддержки научной, научно-технической и инновационной деятельности Энергия без границ</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83813635</t>
+          <t>https://hh.ru/vacancy/83080852</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Знали  Python&lt;/highlighttext&gt;. Работали с MySQL. Работали с Git. Работали с Django. Работали с Linux. Знали ООП. Знали, что такое REST. </t>
+          <t>Высшее образование (электроэнергетика, теплоэнергетика, энергетическое строительство). Опыт проведения акселерационных программ, конкурсов, воркшопов, хакатонов, владение методологией акселерации, анализ эффективности акселерационных и...</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="H12" t="n">
-        <v>60000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>83800127</v>
+        <v>83776307</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Инженер-программист junior</t>
+          <t>Главный специалист по эксплуатации (энергетик)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -887,33 +887,33 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ИНИТИ</t>
+          <t>Росводоканал,ООО</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83800127</t>
+          <t>https://hh.ru/vacancy/83776307</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Опыт программирования на любом из языков ООП (C++,  python&lt;/highlighttext&gt;, perl, java и т.д.). Опыт работы с ОС Linux. </t>
+          <t>Опыт работы в консалтинге - обязательно! Опыт работы в производственно-технических отделах, желательно по направлению водоснабжения/водоотведения. Развитые коммуникабельные навыки, аналитический...</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>30000</v>
+        <v>150000</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>83494438</v>
+        <v>83690286</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Backend разработчик (Python, Junior), удаленно</t>
+          <t>Помощник руководителя</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -923,21 +923,21 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Дунаев Михаил Алексеевич</t>
+          <t>НЕД</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83494438</t>
+          <t>https://hh.ru/vacancy/83690286</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Опыт коммерческой работы на позиции backend-разработчика от полугода. Знания  Python&lt;/highlighttext&gt;3, SQL и фреймворка Django. Опыт работы с библиотекой...</t>
+          <t xml:space="preserve">Высшее образование. Опыт работы от 2-х лет. Владение офисным ПО (Excel, Word, текстовые, табличные и графические редакторы). </t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>30000</v>
+        <v>150000</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -945,11 +945,11 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>82904137</v>
+        <v>83085615</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Разработчик Python</t>
+          <t>Помощник бухгалтера</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -959,33 +959,33 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>EFT GROUP</t>
+          <t>АНО ДПО Академия Медицинского Образования</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/82904137</t>
+          <t>https://hh.ru/vacancy/83085615</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t xml:space="preserve">хорошее знание  Python&lt;/highlighttext&gt; и фреймворков: Flask, Django, FastAPI. - понимание принципов микросервисной архитектуры. - понимание работы веб-сервера. - знание GitFlow. - </t>
+          <t xml:space="preserve">Образование высшее или средне-специальное профильное (желательно по специальности "Бух. учёт, анализ и аудит"). Умение работать в режиме многозадачности. </t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>30000</v>
+        <v>45000</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>83406279</v>
+        <v>83620762</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Middle golang разработчик</t>
+          <t>Ведущий специалист по международной деятельности</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -995,33 +995,33 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>CRTEX</t>
+          <t>Наука и Инновации</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83406279</t>
+          <t>https://hh.ru/vacancy/83620762</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Опыт коммерческой разработки на Go от 2-х лет (или коммерческая разработка на C++/  Python&lt;/highlighttext&gt;/Java и желание перейти на...</t>
+          <t>Образование высшее (международные отношения, мировая экономика, юриспруденция, маркетинг, техническое образование в сфере ядерной  энергетики&lt;/highlighttext&gt; и технологии, ядерных реакторов и материалов...</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>300000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>83185391</v>
+        <v>83956581</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Junior Аналитик</t>
+          <t>Секретарь</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1031,33 +1031,33 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Доценко Дарья</t>
+          <t>Объединенная двигателестроительная корпорация, управляющая компания</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83185391</t>
+          <t>https://hh.ru/vacancy/83956581</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Интерес к теме. Внимательность, любопытство. Коммерческий опыт работы аналитиком не требуется.</t>
+          <t>Образование высшее. Уверенный пользователь ПК (MS Office). Пунктуальность, исполнительность, вежливость, грамотная речь, организаторские способности.</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>84000</v>
       </c>
       <c r="H17" t="n">
-        <v>300000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>83966648</v>
+        <v>83080876</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Python разработчик (Django)</t>
+          <t>Эксперт</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1067,33 +1067,33 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Hammer Systems</t>
+          <t>Фонд поддержки научной, научно-технической и инновационной деятельности Энергия без границ</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83966648</t>
+          <t>https://hh.ru/vacancy/83080876</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Основное - желание развиваться, стрессоустойчивость, готовность к плотной работе. Знание  Python&lt;/highlighttext&gt;. Знание Django, DRF. Знание SQL. REST API. Наличие завершенных проектов. </t>
+          <t>Высшее образование (электроэнергетика, теплоэнергетика, энергетическое строительство). Опыт проведения акселерационных программ, конкурсов, воркшопов, хакатонов, владение методологией акселерации, анализ эффективности акселерационных и...</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>50000</v>
+        <v>84000</v>
       </c>
       <c r="H18" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>83664059</v>
+        <v>82926747</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Junior программист/разработчик Frontend backend/Junior разработчик</t>
+          <t>Менеджер по сопровождению (удаленно)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1103,33 +1103,33 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>AVPOWER</t>
+          <t>ChinaToday</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83664059</t>
+          <t>https://hh.ru/vacancy/82926747</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Увлечение микроэлектроникой, мы работаем с ARM, esp32 и т.д. Знание Linux,  Python&lt;/highlighttext&gt;, C++. Работа в Git. </t>
+          <t>не указано</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>50000</v>
+        <v>80000</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>83756975</v>
+        <v>84085104</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Младший аналитик (IT)</t>
+          <t>Менеджер проектов в нефтегазовой отрасли</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1139,33 +1139,33 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Olima</t>
+          <t>RedStone Capital</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83756975</t>
+          <t>https://hh.ru/vacancy/84085104</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Опыт работы в данной сфере необязателен. Перед трудоустройством проводится подготовка. Приветствуются базовые знания SQL, Java,  Python&lt;/highlighttext&gt;, C#, JavaScript, PHP.</t>
+          <t>Опыт работы по разработке продукции, управлению междисциплинарными проектами в одной из следующих отраслей: нефтегазовая, химическая, медицинская, водное хозяйство, возобновляемая  энергетика&lt;/highlighttext&gt;...</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>140000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>83968218</v>
+        <v>84097043</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Младший разработчик</t>
+          <t>Pentest</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1175,17 +1175,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Первая Грузовая Компания</t>
+          <t>Системный оператор Единой энергетической системы</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83968218</t>
+          <t>https://hh.ru/vacancy/84097043</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Опыт работы в качестве разработчика ПО от 1 года. Фундаментальные знания языка  Python&lt;/highlighttext&gt;, умение писать. Поддерживаемый, читаемый и тестируемый код. </t>
+          <t>Высшее образование ИБ/ИТ, либо незаконченное высшее в этой же сфере. Знание принципов организации сетей передачи данных, принципов функционирования протоколов...</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1197,11 +1197,11 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>82841724</v>
+        <v>83961031</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Junior/Middle backend разработчик на Fast API (Python)</t>
+          <t>Главный бухгалтер (строительство)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1211,33 +1211,33 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Webtronics</t>
+          <t>Наука-Связь</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/82841724</t>
+          <t>https://hh.ru/vacancy/83961031</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Уверенные знаниями языка и стандартных библиотек  Python&lt;/highlighttext&gt; 3. Умение писать качественный и эффективный код на  Python&lt;/highlighttext&gt; 3. Твердый опыт разработки...</t>
+          <t>Опыт работы главным бухгалтером в строительной (строго) организации от 5 лет. Знание всех участков бухгалтерии. Опыт подготовки налоговой и бухгалтерской...</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>82839132</v>
+        <v>82998360</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Удаленный стажер 3d моделирование + computer vision</t>
+          <t>3D Artist (GameDev)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1247,17 +1247,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>MindSet</t>
+          <t>КИБЕР-РОМ</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/82839132</t>
+          <t>https://hh.ru/vacancy/82998360</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Профильное техническое образование, желание развиваться в области компьютерного зрения. Построение классических моделей. Навыки:  Python&lt;/highlighttext&gt;, знание основ ML, знание основ CV. </t>
+          <t>Опыт работы от 5 лет. Портфолио с примерами работ. Профессиональное владение программами моделирования. Опыт работы с Blender. Знание пайплайна производства...</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1269,11 +1269,11 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>83799646</v>
+        <v>82853767</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Аналитик (junior)</t>
+          <t>Инженер-энергетик</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1283,17 +1283,17 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Коннективити Солюшнз</t>
+          <t>ВсеИнструменты.ру</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83799646</t>
+          <t>https://hh.ru/vacancy/82853767</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Опыт работы с базами данных (особенно PostgreSQL) и  Python&lt;/highlighttext&gt; – это плюс. Знание других языков программирования будет являться плюсом. </t>
+          <t>Высшее техническое образование. Понимание операционной деятельности складов. Знания в области пожарной безопасности, слаботочных систем и электрики. Умение грамотно составить техническое...</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1305,11 +1305,11 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>84021559</v>
+        <v>83961718</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Backend разработчик (Python)</t>
+          <t>Офис-менеджер / ассистент руководителя</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1319,33 +1319,33 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Softline</t>
+          <t>S1 | HOLDING (ООО Управляющая Компания Амитс)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/84021559</t>
+          <t>https://hh.ru/vacancy/83961718</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Restful API (Fastapi). Dask, celery, sqlalchemy. Веб-фреймоворки (aiohttp/fastAPI/flask/Django). Асинхронное программирование, работа с микросервисной архитектурой. </t>
+          <t>Стабильный опыт работы в качестве секретаря и/или офис-менеджера/ассистента руководителя от 1 года. Уверенное владение компьютером, MS Office...</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>83644516</v>
+        <v>83953841</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Backend-разработчик Python</t>
+          <t>Помощник руководителя проекта</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1355,33 +1355,33 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Spider Group</t>
+          <t>МОЭСК - Инжиниринг</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83644516</t>
+          <t>https://hh.ru/vacancy/83953841</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Коммерческий опыт программирования на  Python&lt;/highlighttext&gt; от 2 лет. Опыт работы с Django. Опыт работы с облачными сервисами(AWS, Google, Yandex...</t>
+          <t xml:space="preserve">...области строительства,  энергетики&lt;/highlighttext&gt;. Стаж работы - 3 года на инженерно-технических должностях в организациях осуществляющих строительство, реконструкцию в области  энергетики&lt;/highlighttext&gt;. </t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>130000</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>130000</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>83738948</v>
+        <v>83779862</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Тестировщик</t>
+          <t>Frontend developer (React)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1391,33 +1391,33 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>АШАН Ритейл Россия</t>
+          <t>КИБЕР-РОМ</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83738948</t>
+          <t>https://hh.ru/vacancy/83779862</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Знание языков программирования Java и/или JavaScript ( Python&lt;/highlighttext&gt; - будет плюсом). Знание методологии BDD и умение применять. Жизненный цикл разработки программного...</t>
+          <t>Практический опыт работы с нашим стеком технологий. Опыт коммерческой разработки на React от 2 лет. Любознательность и ответственность.</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>180000</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>83952665</v>
+        <v>83525548</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>QA инженер / Тестировщик</t>
+          <t>Главный энергетик</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1427,21 +1427,21 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Ostec</t>
+          <t>М-ГРУПП</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/83952665</t>
+          <t>https://hh.ru/vacancy/83525548</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Понимание процесса разработки ПО и средств тестирования (виды и методы). Знание языка программирования  Python&lt;/highlighttext&gt;. Владение английским языком на уровне чтения...</t>
+          <t>Нам нужен амбициозный человек, который готов реализовать накопленные профессиональные знания и навыки на совершенно новой площадке!!! Тем самым подтвердить свой...</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>180000</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -1449,11 +1449,11 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>84014204</v>
+        <v>78509929</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Python-разработчик</t>
+          <t>Ведущий специалист (Отдел ЕИРЦ по ЮАО)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1463,21 +1463,21 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>КРОК</t>
+          <t>ГБУ ЕИРЦ города Москвы</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/84014204</t>
+          <t>https://hh.ru/vacancy/78509929</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Уверенное знание  Python&lt;/highlighttext&gt;. Понимание основ работы сети и Linux: TCP/IP, HTTP, DNS, файловая система. Опыт работы с языками, инструментами...</t>
+          <t>Наличие высшее или среднее профессиональное (техническое) образование. Стаж работы в области  энергетики&lt;/highlighttext&gt; не менее 1 (одного) года. Знание ПК, (MS...</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>180000</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -1485,11 +1485,11 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>82928430</v>
+        <v>83762965</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Python developer</t>
+          <t>Стажер в рекламное агентство</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1499,33 +1499,33 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>CoMagic.dev</t>
+          <t>i.com</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/82928430</t>
+          <t>https://hh.ru/vacancy/83762965</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Коммерческий опыт разработки на  Python&lt;/highlighttext&gt; на фреймворках Aiohttp/ Aioamqp – от 2 лет. Понимание базовых принципов работы API. Отличное понимание ООП. </t>
+          <t>Свой ноутбук. Желание расти и развиваться в рекламном агентстве.</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>46163376</v>
+        <v>83386492</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Ночной специалист службы технической поддержки (Яндекс Браузер)</t>
+          <t>Эксперт по энергетике в нефтегазовой промышленности</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1535,33 +1535,33 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Яндекс</t>
+          <t>Sitronics Group</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/nochnoj-specialist-sluzhby-tehnicheskoj-podderzhki-46163376.html</t>
+          <t>https://hh.ru/vacancy/83386492</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Для помощи по вопросам десктопной версии  Яндекс Браузера  разыскивается человек, который умеет не только выйти в интернет, но и знает, как потом не принести из него что-то вредное. Ваши сверхспособности понадобятся, чтобы знакомить пользователей с полезными возможностями Браузера. Например, рассказывать, как настроить фильтр рекламы или синхронизировать настройки Браузера на нескольких устройствах. Если вы из тех, кому любопытно разбираться, почему что-то не работает, и нравится помогать людям, присоединяйтесь.  Что нужно делать:   отвечать на сообщения пользователей по почте и в чатах;  консультировать их о вопросах, связанных с Яндексом;  передавать информацию разработчикам и менеджерам, помогая улучшать сервисы;  иногда решать новые интересные задачи — ведь мы постоянно растем и меняемся.   Мы ждем, что вы:   грамотно пишете по-русски;  умеете четко и структурированно излагать мысли;  легко находите главную информацию в текстах разного объема;  умеете читать языки JavaScript, HTML и Python;  имеете высшее или неоконченное высшее образование (техническое будет плюсом);  помогали людям онлайн;  умеете работать самостоятельно и в команде;  готовы к гибкому графику;  ответственны, стрессоустойчивы, самоорганизованны;  умеете работать с большим объёмом информации;  готовы учиться;  не устаете от однообразных задач.   Условия:   работа из дома;  два варианта оформления:  частичная занятость (работа по совместительству) — 5 дней в неделю по 4 часа, можно совмещать с учебой или другой работой;  полная занятость (основное место работы) — 5 дней в неделю по 8 часов;  гибкий график: плавающие выходные, начало смен обсуждается индивидуально;  сдельная оплата, зависящую от количества и сложности задач, которые вы выполните в течение месяца. В среднем — от 18000 рублей в месяц при работе 20 часов в неделю и от 45000 рублей в месяц при работе 40 часов в неделю. Премия по итогам месяца до 30 процентов;  доплата 20% в ночные часы (с 10 вечера до 6 утра);  удаленное оплачиваемое обучение.  </t>
+          <t>Опыт работы на объектах ЛУКОЙЛ, Газпромнефть, Роснефть, Транснефть. Опыт работы не менее 5 лет на инженерной должности в области  энергетики&lt;/highlighttext&gt;...</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>18000</v>
+        <v>20000</v>
       </c>
       <c r="H31" t="n">
-        <v>45000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>45842844</v>
+        <v>46828641</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Инженер-программист встраиваемых систем</t>
+          <t>Старший инженер-энергетик</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1571,33 +1571,33 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Friendwork</t>
+          <t>Филиал ФКУ Налог-Сервис ФНС России по ЦОД в г.Москве</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/inzhener-programmist-vstraivaemyh-sistem-45842844.html</t>
+          <t>https://www.superjob.ru/vakansii/starshij-inzhener-energetik-46828641.html</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Обязанности:    Участие в разработке систем гиростабилизации подвижных объектов.   Написание программного кода для управления двигателями систем стабилизации.   Разработка и реализация алгоритмов систем гиростабилизации.   Разработка встроенного ПО для микроконтроллеров типа STM32.   Реализация взаимодействия с периферийными устройствами по стандартным интерфейсам (RS232, UART, RS485, SPI, I2C, Ethernet и т. п.).   Требования:    Высшее профессиональное (техническое) образование.   Знание С/С++.   Опыт работы с микроконтроллерами типа STM32 и микрокомпьютерами.   Базовое знание ОС семейства Linux.   Понимание работы систем гиростабилизации.   Опыт работы с двигателями (программно-аппаратное сопряжение).   Использование орг. техники (персональный компьютер, печатающие устройства, сканеры, брошюратор).   Знание языка Python является плюсом.   Чтение принципиальных электрических схем и знание Altium Designer является плюсом.   Базовое знание английского, достаточное для свободного чтения документации иностранных компонент.   Уверенное знание теоретической механики и радиотехники на уровне программы профильных ВУЗов.   Коммуникабельность, внимательность к деталям, способность к саморазвитию.   Условия:     Работа в ведущем техническом вузе страны, в городе Долгопрудный (Рядом со станцией Новодачная МЦД-1, или 15 минут от метро Алтуфьево или Ховрино).   Оформление в соответствии с ТК РФ, официальная заработная плата.   Возможности профессионального развития.   Оплачиваемый отпуск, больничный лист.   График работы: 5/2, с 09:00 до 18:00, возможно работа в удаленном режиме.   Заработная плата: от 100 000 рублей.   Молодой активный коллектив.   Возможность бесплатного посещения бассейна и тренажерного зала.   В соответствии с ТК РФ (ст.331), работники сферы образования обязаны предоставить справку о наличии (отсутствии) судимости и (или) факта уголовного преследования, срок изготовления которой может быть до 30 дней, просим заранее позаботиться о её получении.  </t>
+          <t xml:space="preserve"> ФФКУ Налог-Сервис ФНС России - это продвинутая IT - организация с новейшим оборудованием и современными технологиями. Мы занимаемся сопровождением IT - инфраструктуры центров обработки данных (ЦОД) налоговой службы. Наша организация крупнейшая в Европе локальная сеть с 4-мя центрами обработки данных, которая реализует уникальные проекты федерального масштаба с интересными задачами.   Обязанности:    Организация обучения и аттестации электротехнического персонала по знанию требований правил по охране труда при эксплуатации электроустановок.   Проведение инструктирования, проверки знаний и допуска к самостоятельной работе электротехнического персонала.   Контроль правильности допуска персонала строительно-монтажных и специализированных организаций к работам в действующих электроустановках.   Ведение учета и анализа нарушений техники безопасности при работе в электроустановках, несчастных случаев и принятие мер по устранению причин их возникновения.   Организация работы по планированию расходов денежных средств для проведения мероприятий, обеспечивающих выполнение требований охраны труда и электробезопасности, промбезопасности.   Обеспечение пересмотра инструкций и схем.   Ведение делопроизводства по направлениям охраны труда и электробезопасности.   Осуществление контроля за соблюдением в подразделениях Учреждения законодательных и иных нормативных правовых актов по охране труда, оказывать необходимую помощь в организации охраны труда и электробезопасности ответственным за данные направления в филиалах.   Проведение совместно с другими подразделениями Учреждения подготовительной работы по проведению специальной оценки условий труда рабочих мест, выявление не аттестованных рабочих мест.   Участие в проведении оценки профессиональных рисков, подготовке СУОТ.   Оказание подразделениям (филиалам) Учреждения методической помощи в составлении списков профессий и должностей, в соответствии с которыми работники должны проходить обязательные медицинские осмотры.    Требования:    Внимательность;    Умение планирования рабочего времени;   Работа в режиме многозадачности.   Условия:   Достойный уровень "белой" заработной платы, обсуждается с успешным кандидатом;   Оформление строго в соответствии с ТК РФ;   График работы 5/2: с 9.00 до 18.00;   Основной отпуск 28 календарных дней, дополнительный отпуск за ненормированный рабочий день;   Ежегодная материальная помощь к отпуску;   Медицинское обслуживание в ведомственной поликлинике ФНС России для сотрудников и членов их семей;   Возможность отдыха с семьей по льготным ценам в оздоровительных учреждениях ФНС России, детские летние оздоровительные лагеря.    Уважаемые соискатели, просьба в сопроводительном письме указывать Ваши ожидания. </t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>46759846</v>
+        <v>37710150</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Старший аналитик данных в CRM (Отдел анализа эффективности некредитного направления)</t>
+          <t>Инженер КИПИА / энергетик</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1607,21 +1607,21 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Банк ВТБ (ПАО)</t>
+          <t>Сигма Тек</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/starshij-analitik-dannyh-v-crm-46759846.html</t>
+          <t>https://www.superjob.ru/vakansii/inzhener-kipia-37710150.html</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Обязанности:    аналитическая поддержка бизнес-подразделения, развитие и накопление экспертизы в области аналитики, статистики;   анализ эффективности работы CRM, оценка кампаний, подведение итогов пилотов;   участие в крупных аналитических проектах розничного CRM;   поиск решения проблем: увеличения отклика на предложения CRM, расширения охвата базы клиентов предложениями, повышения эффективности процессов;   проведение оценки клиентской базы: анализ жизненного цикла клиентов, прогнозирование поведения, построение клиентского портрета, взаимодействие с data scientists в рамках задач по анализу данных и моделированию;   подготовка бизнес рекомендаций в рамках активностей департамента по результатам проведенных исследований, визуализация результатов исследований;   сопровождение текущей отчетности и создание новой, разработка dashboard, инструментария для контроля деятельности CRM;   разработка инструментария для контроля деятельности CRM.    Требования:    высшее образование (математика, физмат, экономика, статистика);   опыт работы в крупной компании (банки, телеком, retail) в подразделении аналитики от 1 года;   отличное знание SQL (написание сложных запросов, знание оконных функций) - обязательно;   уверенный пользователь MS Office (Excel, P.Point);   опыт использования инструментов BI будет плюсом;   знание python для целей аналитики данных будет плюсом;   опыт анализа больших объемов данных;   наши аналитики, как правило, используют SQL, но мы не ограничиваем специалистов в выборе инструментария;   аналитический склад ума;   умением структурированно излагать мысли, презентовать результаты своей работы.    Условия:    трудоустройство согласно Законодательству;   конкурентная заработная плата;   профессиональное обучение и развитие;   добровольное медицинское страхование, льготные условия кредитования;   корпоративная пенсионная программа, материальная помощь;   спортивная жизнь и корпоративные мероприятия;   возможность построить карьеру в ведущем банке России.   </t>
+          <t xml:space="preserve"> Обязанности:   Обслуживание силовых систем (ВРУ‚ ЩР и др.)‚ систем автоматизации и управления технологическими процессами .   монтаж оборудования;  поиск поломок и их причин, устранение обнаруженных неисправностей;  работа с персоналом (обучение, лекции, техника безопасности);  графики обслуживания, ремонта, замены оборудования и комплектующих;  выполнение работ, необходимых для нормального функционирования оборудования;    разработка технологических схем, модернизация, проектирование;  анализ поломок: причины, способы устранения, профилактика;    -монтажные работы различных средств измерения, систем управления и контроля    Требования    Опыт работы по специальности не менее 3-х лет. Допуск по эл. безопасности Без вредных привычек     Условия:    График работы 5/2 с 9-00 до 18-00. Официальное трудоустройство по Тк Рф, оплата больничных, отпуск 28 дней в году.   </t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>85000</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1629,11 +1629,11 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>46781769</v>
+        <v>46115403</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Аналитик данных (Управление Сквозные бизнес-компоненты)</t>
+          <t>Главный энергетик</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1643,17 +1643,17 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Банк ВТБ (ПАО)</t>
+          <t>Русклимат</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/analitik-dannyh-46781769.html</t>
+          <t>https://www.superjob.ru/vakansii/glavnyj-energetik-46115403.html</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Обязанности:    создавать, развивать и поддерживать регулярную отчетности для топ-менеджмента;   создавать Ad-hoc аналитические отчеты для проверки продуктовых гипотез по запросу руководства;   генерировать и проверять статистические гипотезы;   определять ключевые метрики по новым фичам, прогнозировать как они увеличатся после запуска фичи и следить за их выполнением;   создавать системы аналитических бордов по клиентским и продуктовым метрикам в BI системах.    Требования:    знание Teradata, Hadoop, DBeaver, Bigquery, Python, PyCharm, JupyterHub, Yandex Metrica, AppMetrica, PowerBI, QlickSense;   знание SQL (сложные запросы, оконные функции);   знание python (библиотеки для аналитиков, pyspark);   опыт построения бордов(powerbi, qlick sense);   опыт работы в Yandex Metrica и AppMetrica;   знание основных продуктовых метрик и как их считать;   будет плюсом умение строить модели ML.    Условия:    трудоустройство согласно Законодательству;   конкурентная заработная плата;   профессиональное обучение и развитие;   добровольное медицинское страхование, льготные условия кредитования;   корпоративная пенсионная программа, материальная помощь;   спортивная жизнь и корпоративные мероприятия;   возможность построить карьеру в ведущем банке России.   </t>
+          <t xml:space="preserve"> Должностные обязанности:   Бесперебойное обеспечение энергоресурсами предприятия;  Организация работы ремонтного персонала, контроль выполнения поставленных задач;  Контроль, подготовка проектов и выполнение работ по подключению (газ, вода, электричество, воздух);  Выполнение работ по проверке приборов учета, внедрение календарного плана проверок;  Ведущая роль в расследовании случаев остановки оборудования по причинам отсутствия энергии, разработка и выполнение мер по их предотвращению;  Контроль выполнения ППР для вентиляционного, теплоснабжающего и энергетического оборудования, организация работ по ремонту;  Организация и контроль выполнения работ подрядными организациями по вопросам энергетики;  Составление заявок на приобретение оборудования, материалов, зап. частей;  Подготовка проектов по снижению затрат, защита и внедрение.   Требования:   Высшее или среднее специальное профильное образование;  Опыт работы не менее 3 лет;  Владение программами MS (office);   Условия:   Работа на ведущем заводе по производству радиаторов отопления «Royal Thermo» в Технопарке «Русклимат-ИКСЭл», г. Киржач, Владимирской области.  Возможности увеличения дохода:  акция «Приведи друга» - 8.000 руб. за каждого пришедшего по Вашей рекомендации нового работника;  предложения по повышению эффективности производства - от 2.500 руб. до 5 000 руб. за каждое предложение.  Официальное трудоустройство, «белая» заработная плата - 2 раза в месяц всегда вовремя, оплачиваемые отпуск и больничные листы;  Качественные спецодежда и рабочий инструмент;  Доставка корпоративным транспортом (г. Кольчугино, г. Александров, г. Карабаново, п. Белая Речка);  График работы сменный: 5/2.  </t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1665,11 +1665,11 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>38671598</v>
+        <v>46165480</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Системный администратор</t>
+          <t>Энергетик</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1679,33 +1679,33 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>ЭКО центр</t>
+          <t>Нефтегазсервисстрой</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/sistemnyj-administrator-38671598.html</t>
+          <t>https://www.superjob.ru/vakansii/energetik-46165480.html</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Требования:   Наши ожидания: - Вы знаете что такое кластер виртуализации Proxmox (kvm) и понимаете, как он работает.  - Вы уверенно знаете, как администрировать операционные системы Linux (debian, CentOS, Windows) - Вы осознаете принципы работы современной сетевой инфраструктуры и стека TCP/IP, принципы сетевого взаимодействия систем, знаете, что такое Firewall, NAT и прочие странные слова, зачем нужны VLAN и как маршрутизировать трафик средствами OPNsense и Mikrotik. А самое главное зачем и куда!! - Вы знаете как настроить отправку почтовых голубей через сервер Zimbra - Вы знаете что такое Zabbix и сможете настроить мониторинг всего чего угодно.  - Вы знаете для чего нужно серверное железо и что куда воткнуть, что такое RAID (hardware, software).  - Вы знаете что такое AD, DNS, DHCP, как работают и настраиваются групповые политики.  - Вы знаете что такое СХД (Qnap, Windows SMB) и умеете настраивать и администрировать.  - Вы стремитесь автоматизировать рутинные IT процессы, поэтому знаете, как это сделать.  - Вы знаете как работать с IP телефонией (Asterisk), как правильно раскидать звонки и сделать красивое голосовое приветствие (сложный IVR).  - Вы знаете как работать с пользователями и пользовательскими ОС. У Вас крайне высокий уровень стрессоустойчивости.  - Вы понимаете, что выполнение поручений руководителя — это крайне важно.  Будет огромным плюсом если Вы: - Умеете работать с БД Postgresql, MySQL - Знаете, как писать скрипты на bash, python, php (желательно PowerShell) - Знаете, что такое СКУД и IP видеонаблюдение и умеете с этим работать.  - Умеете самостоятельно администрировать часть инфраструктуры и отдельные проекты.  - Знаете как улучшить показатели производительности и отказоустойчивости сервисов в непосредственной зоне ответственности, предложить варианты оптимизации инфраструктуры.  - Знаете как осуществить мониторинг сервисов, выявить проблемные места, устранить неисправности и задокументировать проблему. Оперативное реагировать на оповещения и сигналы тревоги. Эскалация проблем.  - Понимаете, что рабочий процесс может затянуться и придется задержаться на работе.   Требования: - Высшее образование. - Коммуникабельность, доброжелательность. - Ответственность, стрессоустойчивость, способность быстро усваивать новую информацию. - Умение работать в режиме многозадачности. - Грамотная речь.   Условия   - Работа в крупной медицинской, динамично развивающейся Компании. - Строгое соблюдение Трудового законодательства, своевременная и в полном объеме выплата заработной платы, премии, скидки на медицинские услуги , оказываемые в нашей организации. - Современное медицинское оборудование, комфортные условия труда. - Обучение и развитие в Компании. - График работы: гибкий с 8-00 до 20-00 с плавающими выходными днями. - Недалеко от метро Нагорная, Профсоюзная, Тульская, Нижние Котлы. - Будем рады видеть Вас в нашем дружном коллективе!!!   </t>
+          <t xml:space="preserve">Обязанности:  Подключение/отключение бытовых вагончиков в вахтовом городке, учет расхода электроэнергии, ведение журналов по электробезопасности, подготовка и сдача аттестации по ПБ, участие в комиссии по проверке знаний электробезопасности у рабочих с записью в спец,журнале проведения инструктажей. Ремонт и наладка бензогенераторов, УШМ, сварочных аппаратов. Монтаж средств ЭХЗ, ведение и сдача исполнительной документации по монтажу ЭХЗ заказчику и др.  Требования:  Опыт аналогичной работы.  Наличие 5 гр. электробезопасности.  Знание высоковольтных и малоточных сетей, опыт работы на трассе газопровода с ДЭС-100,150,200, с очистным комбайном. Ремонт и наладка бензогенераторов, УШМ, сварочных аппаратов. Монтаж средств ЭХЗ, ведение и сдача исполнительной документации по монтажу ЭХЗ заказчику и др.  Условия: Вахтовый метод работы. Вахта 2 месяца через месяц. Шестидневная рабочая неделя с понедельника по субботу с 08.00-19.00 (перерыв на обед с 12.00-13.00) .  Оформление по ТК РФ. Все социальные гарантии. Оплата проезда до места работы. Предоставляем бесплатное жилье (общежитие). Бесплатные обеды. </t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>120000</v>
+        <v>118000</v>
       </c>
       <c r="H35" t="n">
-        <v>120000</v>
+        <v>118000</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>41239513</v>
+        <v>46165495</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Старший научный сотрудник</t>
+          <t>Инженер-энергетик</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1715,17 +1715,17 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ФГБОУ ВО МГППУ</t>
+          <t>Лаборатория Гемотест</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/starshij-nauchnyj-sotrudnik-41239513.html</t>
+          <t>https://www.superjob.ru/vakansii/inzhener-energetik-46165495.html</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Уважаемые коллеги, при Министерстве просвещения РФ на базе ФГБОУ ВО МГППУ создан  Федеральный координационный центр по обеспечению психологической службы в системе образования РФ . Мы ищем старшего научного сотрудника, который умеет работать с большим объёмом данных и грамотно обрабатывать информацию с помощью различных инструментов анализа.   Вашими основными задачами будут:    Участие в разработке, апробации, экспертизе передовых технологий и механизмов работы, направленных на: создание психологически безопасной развивающей образовательной среды; сохранение психологического здоровья и благополучия всех субъектов образовательного процесса; индивидуализацию обучения и воспитания; снижение рисков негативной социализации обучающихся.   Проведение научных исследований и разработок в интересах развития психологической службы в системе образования.    Разработка планов и методических программ проведения исследований.    Организация сбора и изучение научно-технической информации по теме, проведение анализа и теоретическое обобщение научных данных и результатов исследования.    На основании результатов исследований подготовка методических рекомендаций.   Участие в организации и проведении научных мероприятий (конференций, симпозиумов, семинаров, совещаний, круглых столов и др.): методическая, информационная, организационная поддержка в обеспечении проведения научных мероприятий. Публикация материалов исследований, участие в научных мероприятиях всероссийского и международного уровней.    Требования к кандидату:    Высшее психологическое образование;   Наличие ученой степени: кандидат психологических наук;   Опыт проведения научных исследований и описание результатов;   Опыт работы практическим психологом в сфере образования;   Владение современными цифровыми инструментами (Microsoft Office, Google-Форм и др.);   Работа со статистикой и аналитикой;   Опыт работы в обработке количественных данных средствами Excel и/или R и/или Python и/или SPSS;   Знание современных психолого-педагогических методов работы психологической службы;   Английский язык не ниже среднего В1 (Intermediate);   Нам важно Ваше стремление к развитию и активная жизненная позиция.    Что мы предлагаем:    Оформление в соответствии с ТК РФ;   Стабильная официальная заработная плата;   Работа в мотивированной профессиональной команде, нацеленной на результат;   Дружный коллектив.   </t>
+          <t xml:space="preserve"> Гемотест — российская медицинская компания, оказывающая услуги в сфере лабораторной диагностики. Созданная в 2002 году, она продолжает активно развиваться — совершенствовать бизнес-процессы, расширять спектр выполняемых исследований и географию присутствия. Сегодня отделения Гемотест открыты более чем в 700 городах в России, Киргизии, Таджикистане и Казахстане, а ее услугами ежегодно пользуются более 11 миллионов пациентов.  Мы видим свою миссию в развитии социально-ответственного бизнеса и стремимся выстраивать продуктивное и долгосрочное партнерство с каждым сотрудником компании.  Присоединяйтесь к команде Гемотест!  Лаборатория «Гемотест» – один из лидеров коммерческой лабораторной диагностики в России.  С 2003 года мы открыли более 850 лабораторных отделений в более чем 350 городах РФ, Киргизии и Таджикистана.  Каждый год «Гемотест» выполняет более 55 миллионов тестов для 5 миллионов пациентов.  Мы делаем качественную лабораторную диагностику доступной для каждого.  Сейчас у нас открыта вакансия "Инженер-энергетик"  Требования:   Высшее техническое образование по специальности: энергетика, эксплуатация зданий;  Опыт работы электриком, инженером по эксплуатации, энергетиком, мастером РЭС от 3-х лет,  Практические навыки в поиске и устранении неисправностей сложного электротехнического оборудования;  Опыт организации проведения работ в действующих электроустановках;  Знание электроавтоматики и электротехники;  Опыт работы с измерительным оборудованием;  Чтение схем и понимание технической документации;  4 группа по электробезопасности до и выше 1000 В;   Обязанности:   Обеспечение бесперебойной безопасной работы, своевременного технического обслуживания электроустановок, электрических сетей.  Расчет потребностей в электроэнергии и контроль за рациональным потреблением энергоресурсов; взаимодействие с ресурсоснабжающими организациями;  Проверка соответствия схем электроснабжения фактическим эксплуатационным с отметкой на них о проверке; пересмотр инструкций и схем контроль замеров показателей качества электрической энергии.  Ведение технической документации;  Подготовка обоснования технического перевооружения, развития, реконструкции и модернизации электроустановок и электрических сетей организации; участие в испытаниях и приемке электроустановок и электрических сетей в эксплуатацию, в рассмотрении причин аварий энергетического оборудования.   Условия:   Работа в Компании Федерального уровня (клинико-диагностическая лаборатория);  Месторасположение: г. Люберцы, ул. Октябрьский проспект д.183;  Оформление по ТК РФ;  График работы 5/2 с 9:00 до 18:00;  Коллектив профессионалов, любящих свое дело.  </t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1737,11 +1737,11 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>45812126</v>
+        <v>46261524</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Аналитик</t>
+          <t>Инженер-энергетик</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1751,33 +1751,33 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Альпинтех</t>
+          <t>Ремстрой-Алексс</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/analitik-45812126.html</t>
+          <t>https://www.superjob.ru/vakansii/inzhener-energetik-46261524.html</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Перечень задач:    Организация доступности информации для оперативного/тактического/стратегического управления. Проектирование и разработка витрин данных  Разработка аналитической отчетности.  Разработка дашбордов для оперативного и стратегического управления.    Управленческие компетенции    Желательно:  &lt;ol&gt; Опыт управление проектом/ управление продуктом в областях: &lt;/ol&gt;  Управленческая отчетность  Учетные системы  Витрины данных  BI системы    Технические компетенции    BI инструменты и инструменты подготовки данных  Python/Jupiter Notebook  Apache Airflow  Google Sheet + Apps Script  Excel  Системы для управления связками между сервисами (например N8N)  Базы данных  Математика на здоровом уровне  Эстетический вкус в визуализация и презентации данных  Способность задавать вопросы, структурировать и систематизировать.    Условия:     График работы с понедельника - по пятницу, с 8:00 - 17:00 (09:00 до 18:00)  Соблюдение трудового законодательства (официальное оформление с первого рабочего дня, "белая" заработная плата, оплачиваемые отпуска и больничные);  Стабильный рост заработной платы.  Корпоративные подарки от Компании на рождение ребенка, на 23 февраля. Новогодние подарки детям сотрудников.  Корпоративные скидки на нашу продукцию.  </t>
+          <t xml:space="preserve"> Обязанности:   Обеспечивать бесперебойную работу, правильную эксплуатацию, ремонт и модернизацию энергетического оборудования, электрических и тепловых сетей, воздухопроводов и газопроводов.  Определять потребность производства в топливно-энергетических ресурсах, готовить необходимые обоснования технического перевооружения, развития энергохозяйства, реконструкции и модернизации систем энергоснабжения.  Контролировать соблюдение норм расхода топлива и всех видов энергии.  Осуществлять технический надзор за контрольно-измерительными, электротехническими и теплотехническими приборами, применяемыми на предприятии   Требования:   Опыт работы;  Наличие высшего образования;   Готовность к редким командировкам.   Условия:   Оформление по ТК РФ;  Полный соцпакет;  График работы 5/2 с 9:00-18:00, в пятницу до 17:00.  </t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>150000</v>
+        <v>80000</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>45980418</v>
+        <v>46405892</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Преподаватель IT дисциплин / Мастер ПО (Направление IT)</t>
+          <t>Главный энергетик</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1787,21 +1787,21 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ГБПОУ Колледж связи № 54 имени П. М. Вострухина Образовательное подразделение 8</t>
+          <t>Компания СПЛАВ</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/prepodavatel-it-disciplin-45980418.html</t>
+          <t>https://www.superjob.ru/vakansii/glavnyj-energetik-46405892.html</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Обязанности:    Подготовка и проведение занятий, работа с календарными планами, составление планов уроков, ведение учебной документации, контроль знаний учеников.    Требования:    Общие требования    Практический опыт работы с развертыванием, сборкой, настройкой учебных лабораторий. Подключение, установка, настройка сетевого оборудования. Маршрутизация, коммутация локальных сетей. Настройка оконечных рабочих мест пользователей. Установка программного обеспечения. Знание основных сетевых технологий стека TCP/IP. Умение работать с ОС Windows Server, администрирование Active Diretcory, разграничение прав пользователей с помощью групповых политик.        Операционные системы специального назначения  Установка и работа с Astra Linux Special Edition, Astra Linux Directory. Работа с СЗИ Astra Linux (Контроль целостности. Мандатное управление доступом). Доменные политики безопасности. Интеграция DLP-системы на базе ОС Astra Linux, в т.ч. в распределенном режиме. Автоматизация процессов установки ОС и ПО на ОС AstraLinux с помощью Ansible/Vagrant. Приветствуется наличие сертификата ALSE от Учебного центра Astra Linux      Общая инфраструктура для построения лабораторно-учебных стендов  Работа с гипервизорами Virtualbox, VMware workstation, VMWare ESXI. Работа с созданием, настройкой, миграцией виртуальных машин для построения учебных стендов. Администрирование VMWare ESXI, создание пользователей, разграничение областей видимости. Управление виртуальными машинами в автоматическом режиме.      Навыки программирования  Python, C#, работа с запросам SQL. Понимание и применение основных операторов (SELECT, INSERT, UPDATE, DELETE). Типы данных SQL. Работа по созданию таблиц, проектирование баз данных. Составление учебных материалов по Проектированию и управлению БД.  Условия:   Проживание г. Москва.   </t>
+          <t xml:space="preserve"> Компания «СПЛАВ» занимается производством и продажей одежды и снаряжения для туризма, активного отдыха. Мы также работаем в направлении «military» и городской одежды.  Компания на рынке уже 30 лет.  Мы ищем инженера-энергетика с опытом работы.  Обязанности:   Обеспечение эффективной эксплуатации, технического обслуживания и ремонта электроустановок и электрооборудования.  Организация и контроль работы электротехнического персонала.  Технический надзор выполнения электромонтажных работ.  Расчет нагрузок, подбор оборудования.  Ведение технической документации.   Требования:   Образование высшее техническое (профильное).  Опыт выполнения электромонтажных и ремонтных работ.  Знание электротехники (ПУЭ), правил и норм, СНиП.  Умение работать с проектной и сметной документацией.  Знание электротехнического рынка и техническая грамотность.  Наличие организационно-управленческих навыков.  Уверенный пользователь ПК.  Личные качества: активная жизненная позиция, инициативность, скрупулезность.   Условия:   Оформление согласно ТК РФ;  Стабильная заработная плата;  График работы ПН -ПТ с 9:00 - до 18:00  Скидки на продукцию компании;  Корпоративные праздники, туристические слеты;  Дружный коллектив профессионалов в стабильной компании  </t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>85000</v>
+        <v>100000</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -1809,11 +1809,11 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>46185192</v>
+        <v>46552931</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Data Scientist</t>
+          <t>Ведущий инженер-энергетик</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1823,33 +1823,33 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Спортмастер</t>
+          <t>ВИНИТИ РАН</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/data-scientist-46185192.html</t>
+          <t>https://www.superjob.ru/vakansii/veduschij-inzhener-energetik-46552931.html</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Обязанности:    Использовать алгоритмы машинного обучения для решения бизнес-задач   Исследовать данные с целью получения новых признаков   Разрабатывать требования для сбора данных, дизайн A/B тестов   Заниматься написанием эффективного кода для получения агрегатов данных   Развивать инфраструктуру для автоматического построения и использования моделей машинного обучения    Требования:   Высшее техническое образование   Уверенное знание SQL и готовность писать эффективные запросы  Уверенное владение Python (библиотеки работы с данными)  Опыт использования и внедрения алгоритмов машинного обучения  Знание базовых алгоритмов и структур данных, понимание плюсов и минусов   Уверенное знание математической статистики, умение применять для решения задач   Технический английский на уровне чтения статей и участия в конференциях    Условия:   формат работы;  График работы: 5/2; 8.00-17.00, 9.00-18.00 или 10.00-19.00 (на выбор);  Полугодовой бонус;  ДМС - после испытательного срока;  Дисконтная карта на продукцию 30% магазинов сети + корпоративные скидки и специальные условия от партнеров;  Обучение - доступно внутреннее и внешнее обучение, проводим внутренние митапы, техтолки, посещаем профильные конференции;  Некоторые бонусы предоставляются по принципу "кафетерия". Расскажем об этом подробнее при первом контакте.  </t>
+          <t xml:space="preserve"> Службы главного инженера   Обязанности:    Обеспечение бесперебойной работы, ремонт и модернизация энергетического оборудования, электрических и тепловых сетей, воздухопроводов и газопроводов  Составление заявок на приобретение оборудования, материалов, запасных частей, необходимых для эксплуатации энергохозяйства, выполнение расчетов с необходимыми обоснованиями мероприятий по экономии энергоресурсов, потребности подразделений предприятия в электрической, тепловой и других видах энергии, участвует в разработке норм их расхода, режима работы подразделений предприятия, исходя из их потребностей в энергии  Контроль за соблюдением норм расхода топлива и всех видов энергии  Составление графика снижения энергетических нагрузок в часы максимальных нагрузок энергосистемы и обеспечение их выполнения в пределах определенной для подразделения предприятия величины, проведение паспортизации установленных на предприятии энергетических, электрических и природоохранных установок  Участие в испытаниях и приемки энергетических установок и сетей в промышленную эксплуатацию, рассмотрение причин аварий энергетического оборудования и разрабатывает мероприятия по их предупреждению, созданию безопасных условий труда  Организация проверки и испытаний средств релейной защиты и автоматики  Осуществление технического надзора за контрольно-измерительными, электротехническими и теплотехническими приборами, применяемыми на предприятии, а также обеспечение подготовки котлов, сосудов, работающих под давлением, трубопроводов пара и горячей воды, электроустановок и других объектов энергохозяйства для приемки в эксплуатацию, проверки и освидетельствования органами государственного надзора  Осуществление контроля за соблюдением инструкций по эксплуатации, техническому обслуживанию и надзору за энергооборудованием и электрическими сетями  Участие в разработке и внедрении стандартов и технических условий на энергетическом оборудовании  Осуществление контроля за выполнением капитальных и других ремонтов энергооборудования   Требования:   Высшее техническое образование  Знания электрического и силового оборудования  Знания правил эксплуатации электроустановок, правила устройства электроустановок  Наличие электробезопасности не ниже 4 гр.    Условия:    Оформление в соответствии с ТК, испытательный срок 3 месяца  График работы 5/2, с понедельника по четверг с 9.00 до 18.00, в пятницу с 9.00 до 16.45 (суббота, воскресенье, праздничные дни - выходные)  </t>
         </is>
       </c>
       <c r="G39" t="n">
         <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>46505351</v>
+        <v>27313199</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Учитель информатики</t>
+          <t>Инженер-энергетик</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1859,21 +1859,21 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ГБОУ ШКОЛА № 1579</t>
+          <t>Государственный центральный музей современной истории России</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/uchitel-informatiki-46505351.html</t>
+          <t>https://www.superjob.ru/vakansii/inzhener-energetik-27313199.html</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Обязанности:    Проведение уроков.  Работа в ЭЖД.  Подготовка оборудования к урокам.  Участие обучающихся в проектной деятельности, конкурсах, олимпиадах.   Требования:   Наличие профильного образования (технического или педагогического).   Условия:   Дружный коллектив.  Возможность дополнительного обучения.  Наличие современного оборудования.  </t>
+          <t xml:space="preserve"> Мы, команда музея современной истории России - один из крупнейших в мире музеев, посвященных периоду новейшей истории. Работать с нашими посетителями приятно, иногда сложновато, но в тоже время интересно. Мы в поиске лучших сотрудников для расширения нашей дружной команды.     Что нужно делать:    Обеспечение бесперебойной работы, правильной эксплуатации, ремонта и модернизации энергетического оборудования, электрических и тепловых сетей, вентиляции и кондиционирования в зданиях Музея и обособленных отделах;  Определение потребностей Музея в топливно-энергетических ресурсах;  Организация и контроль работы электротехнического персонала в части эксплуатации электрооборудования;  Обеспечение необходимыми комплектующими и материалами для выполнения работ, составление заявок;   Обеспечение работы системы освещения и электрического оборудования в экспозиционных залах и помещениях Музея  Составление энергобаланса, годовых заявок на потребление энергоресурсов;   Выполнение необходимых расчетов по энергоснабжению;   Составление и контроль выполнения графиков планово-предупредительных ремонтов энергооборудования и сетей энергоснабжения;  Учёт и контроль расхода потребляемых ресурсов;  Работа с подрядными организациями;  Взаимодействие с контролирующими, надзорными, энергоснабжающими организациями.    Мы ждем, что Вы:   Имеете высшее профессиональное образование (энергетическое, электротехническое), опыт работы не менее 3 лет в эксплуатации зданий и инженерных систем (электроснабжение, водоснабжение, теплоснабжение, вентиляция, кондиционирование).  Обладаете знаниями норм расхода топливно-энергетических ресурсов, правил приема и сдачи оборудования после монтажа и ремонта, правил эксплуатации зданий и сооружений, правил их эксплуатации, порядка и методов планирования и производства текущих и ремонтных работ, ПТЭЭП, ПУЭ, ПТЭТЭ.    Мы предлагаем:    Оформление в соответствии с Трудовым кодексом Российской Федерации, испытательный срок 3 мес.   Стабильную зарплату на уровне рынка и выплаты на карту без задержек, оплачиваемые отпуска и больничные листы.    Премирование по результатам месяца, квартала, года за эффективную работу.    Работу в историческом здании в центре Москвы.     График работы: 5/2, выходные: суббота, воскресенье.     Преимущества работы в ГЦМСИР:     «Белая» зарплата и надежный работодатель;  Мы заключаем трудовой договор с каждым сотрудником и гарантируем своевременные выплаты;   Возможность стать частью сильной команды и истории, которую создаете Вы.    Присоединяйтесь к нашей дружной команде, мы Вас ждем!   </t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>85000</v>
+        <v>55000</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -1881,11 +1881,11 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>46528737</v>
+        <v>41666804</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Педагог дополнительного образования (Лицей Академии Яндекса)</t>
+          <t>Инженер-энергетик</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1895,33 +1895,33 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Школа № 1210</t>
+          <t>Твой Дом</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/pedagog-dopolnitelnogo-obrazovaniya-46528737.html</t>
+          <t>https://www.superjob.ru/vakansii/inzhener-energetik-41666804.html</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Обязанности:   Осуществляет разнообразную развивающую деятельность обучающихся (воспитанников) в области дополнительного образования.  Комплектует состав кружка, секции, студии, клубного объединения и других форм внеурочной работы с обучающимися и принимает меры по его сохранению в течение срока их работы.  Участвует в разработке и реализации образовательных программ, несет ответственность за качество их выполнения, жизнь и здоровье обучающихся.  Составляет планы и программы занятий, обеспечивает их выполнение.  Выявляет творческие способности обучающихся, способствует развитию их интересов и склонностей.  Организует участие обучающихся в массовых мероприятиях.  Оказывает консультативную помощь родителям (лицам, их заменяющим), а также педагогическим работникам в пределах своей компетенции.  Обеспечивает при проведении занятий соблюдение правил охраны труда и санитарно-гигиенических норм.  Участвует в деятельности методического объединения, самоуправлении учреждения.  Систематически повышает свою профессиональную квалификацию.   Требования:   В Лицей Академии Яндекса на площадку ГБОУ Школа 1210 (2023/2024 учебный год!) требуется педагог дополнительного образования по программе "Учим программировать на Python".     Соискатель должен пройти отбор в преподаватели Лицея Академии Яндекса.   Наличие справки об отсутствии судимости, справки об административных нарушениях за употребление наркотических средств и психотропных веществ.   Условия:    Занятия в группе во второй половине дня, два раза в неделю по 2 часа.       ВНИМАНИЕ: резюме кандидатов, которые не соответствуют требованиям, не рассматриваются.  Просьба в сопроводительном письме указывать наличие пройденного отбора в преподаватели Лицея Академии Яндекса. </t>
+          <t xml:space="preserve">  ТВОЙ ДОМ - не имеющая аналогов по товарному ассортименту, сеть гипермаркетов, входящая в состав крупнейшего российского холдинга CROCUS GROUP. По истине уникальная торговая площадка, сочетающая 7 гипермаркетов под одной крышей! Тысячи брендов. Более 300 тысяч наименований товаров различных категорий: товары для дома, ремонта, дизайна, мебельный салон, оранжерея, гастроном и многое другое. Здесь каждый соискатель найдет для себя сферу для профессионального развития и личностного роста. Стань частью амбициозной команды ТВОЙ ДОМ!    Готовы рассмотреть студентов на данную позицию!   Мы предлагаем:    Оформление по ТК РФ (трудоустройство с 1-го рабочего дня).  График работы: 5/2 (день с 10:00 до 19:00).   "Белая" стабильно выплачиваемая заработная плата (3 раза в месяц).  Дружелюбный, сплоченный коллектив.  Скидки на весь ассортимент магазина (карта лояльности).   Льготное питание для наших сотрудников.   Корпоративный транспорт.  Место работы: м. Медведково, ГП "Твой Дом".    Ваши обязанности:    Организация эксплуатации и своевременного ремонта энергетического оборудования и электросетей, бесперебойное обеспечение производства электроэнергией.  Разработка и составление графиков ППР, контроль их выполнения.  Контроль за рациональным использованием энергоресурсов.  Руководство организацией и планирование работ в электроустановках, разработка графиков ремонта электрооборудования и электросетей.  Модернизация и реконструкция электросетей и оборудования 10 кВ, до 1000В.  Участие в испытаниях и приемке энергоустановок и энергосетей в эксплуатацию.  Контроль за соблюдением правил охраны труда при производстве работ в электроустановках.  Организация разработки мероприятий по экономии энергоресурсов.      Наши ожидания:    Ответственность, внимательность.   Ждем Вас на собеседование в любой будний день с 10:00 до 13:00 или с 14:00 до 17:00. До ГП «Твой Дом» можно добраться: от станций метро до остановки «Твой Дом/Ашан»: - ст. м. Медведково автобусом - 314к; - ст. м. Бабушкинская автобусами - 314к, 197, 567, С15; - ст. м. Бибирево автобусами – 771, 509, 618, 31. От станции Мытищи автобусами - 177, 567, 419 (остановка «Ашан», необходимо перейти через дорогу). В торговом комплексе необходимо обратиться на стойку информации «Сервис-центр». </t>
         </is>
       </c>
       <c r="G41" t="n">
         <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>57500</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>46795750</v>
+        <v>44913359</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Программист Бэкенд AI</t>
+          <t>Инженер-энергетик</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1931,33 +1931,33 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ТЕХТОБ</t>
+          <t>Гроскран</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/programmist-bekend-ai-46795750.html</t>
+          <t>https://www.superjob.ru/vakansii/inzhener-energetik-44913359.html</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Обязанности:   Мы ищем специалиста, способного дополнить команду работающую над разработкой продукта связанного с AI / LLM моделями.  Наша команда состоит из профессионалов, которые успешно получили стартап-пермит в Силиконовой долине, мы создаем продукты на основе LLM. В данный момент мы нацелены на создание интерактивного помощника, обучаемый инструмент для повседневного участия в работе человека и приложения.  Что нужно будет делать в рамках команды:   Проектировать, разрабатывать и внедрять новый продуктовый функционал решений, интеграций, API;  Разработка нового функционала на Python / Django (или С#, C++), приветствуется иметь навыки написания кода на других языках программирования;  Разработка программного обеспечения на базе СУБД PostgreSQL;  Подготовка данных для обучения и тестирования моделей;  Поиск точек роста, узких мест, нахождение путей улучшения качества моделей за счет данных;  Предобработка, фильтрация и сегментация данных;  Выстраивание архитектуры и написание пайплайнов разметки данных;  Проводить тестирование и оптимизацию текущих моделей, работа с метриками;  Оптимизировать существующие решения, в т.ч. архитектурные с точки зрения производительности и надежности;  Довести качество до ChatGPT, помогать решать бизнес задачи приложения с помощью нашей технологии;  Участие в эксплуатации и развитии ИТ-инфраструктуры организации;  Заниматься непрерывным обменом знаниями со всей командой разработчиков;  Регулярное проведение knowledge sharing sessions является частью нашей культуры;  Регулярное проведение статус отчетов (Вторник, Четверг 20:00 - 21:00 мск);  Решение задач в режиме стартапа, ответственность за результат;  Анализ и оптимизация существующего кода;  Рефакторинг текущей кодовой базы, проведение ревью;  Поиск ошибок, их устранение;  Разработка интеграций с различными внешними системами;  Оптимизация сервисов под высокие нагрузки;  Работа с ОС Linux (CentOS, openSUSE и др.), Asta linux, Windows (7,10,11, server 2012 – 2019);   Быть гибким в мышлении, трудолюбивым, жить своим делом. Быть честным и преданным. Не лениться, не быть гордым, быть компромиссным и вежливым, терпеливым. Обеспечить высочайшее качество взаимодействия, выполнять все оперативно. Принимать достойно критику, стараться подстроиться и быть словно единым целым с этим делом.  Требования:  Высшее техническое или неоконченное высшее образование (профильное);   Опыт коммерческой разработки клиент-серверных приложений;  Понимание ООП/GoF/SOLID;  Понимание Natural Language Processing (NLP) , знакомство с LangChain и Large Language Model (LLM) , а также базовый Elastic Search будет плюсом;  Опыт работы с RESTful API, интеграция с внешними сервисами;  Знание основ работы с базами данных, опыт работы с PostgreSQL или MySQL;  Понимание принципов работы машинного обучения, опыт работы с TensorFlow, Keras или PyTorch будет преимуществом;  Отличное знание Python 3, библиотек для разработки API и работы с данными (FastAPI, Pandas, Numpy, SQL Alchemy, asyncio);  Отличное знание подходов CI/CD и их реализации на GitLab;  Отличное знание PostgreSQL;  Уверенное знание .NET, C#;  Опыт построения решений в микросервисной архитектуре;  Работа по задачам с высокой степенью неопределенности;  Опыт постановки задач и сбора требований напрямую от заказчика, без детальной проработки у аналитика. Желание самому предлагать идеи реализации и проявлять инициативу в целом;  Умение работать с системами управления версиями (Git), таск-трекинга;  Умение писать качественные комментарии;  Опыт разработки нагруженных многопользовательских систем;  Опыт работы с данными и алгоритмами, отличное знание SQL, Pandas, FastAPI;  Понимание Deep learning (DL), опыт обучения просто моделей и больших моделей;  Участие в проектировании архитектуры, выработке решений по отказоустойчивости и производительности;  Разработка нового и доработка существующего back-end и front-end функционала;  Ответственность, дисциплинированность, стрессоустойчивость;  Читать техническую документацию на английском языке;   &lt;i&gt;Желательно:&lt;/i&gt;  Умение разбираться в чужом коде;   Понимание работы http, https. REST, RESTful, SOAP;  Опыт работы с highload-сервисами;  Опыт работы с ClickHouse, Pinecone;  Опыт работы с Flask;  Опыт docker/kubernetes, docker-compose;  Опыт создания проектов с "0";  Опыт/понимание математики и геометрии и алгоритмов связанных с математикой и геометрией;  Опыт проектирования и развития высоконагруженных систем;  Опыт работы с MySQL / Postgres;  Опыт работы c redis / rabbitmq;  Опыт управление командой разработчиков;  Желание много работать и учиться;  Разговаривать на английском языке;    Условия:  Дистанционное взаимодействие (как минимум первые 6 месяцев). Вы работаете у себя дома;   Доступно соискателям с инвалидностью;  Достойная заработная плата по результатам собеседования в зависимости от опыта и навыков;  Возможно оформление: договор услуг, подряда, ГПХ, самозанятые, ИП;  Возможна полная занятость 5/2 8 часов (график обсуждаетсяс учётом Ваших пожеланий);  Возможна подработка: сменами по 4-6 часов или по вечерам;  Своевременная выплата зарплаты;  Профессиональная команда единомышленников;  Открытость руководства к изменениям и улучшениям, без бюрократии;  Работая с нами, ты:   Обогатишь свой опыт участия в разработке и запуске приложений/сервисов от идеи до вывода на рынок;  Обретёшь профессиональная команду единомышленников;  Сможешь работать, не выходя из дома;  Станешь созидателем проекта мирового масштаба;  Прокачаешь английский язык;  Получаешь возможности карьерного роста (Компания постоянно развивается и растёт);   На данном этапе мы создаем юридическое приложение и нам важно найти специалиста, который занимался системами обработки текстовой информации, интересуется машинным обучением и способен применять существующие модели, а в перспективе стать ключевым игроком в продуктовой и технической реализации проекта.   Уважаемые соискатели, просьба указывать ожидаемый уровень З/П на руки в сопроводительном письме!   </t>
+          <t xml:space="preserve"> Обязанности:   Организация и обеспечение бесперебойной эксплуатации энергетического хозяйства.  Организация работы по вопросам электробезопасности.  Организация договорной работы с поставщиками энергоресурсов, сетевыми организациями, организациями водопроводно-канализационного хозяйства, теплоснабжающими организациями и с организациями, выполняющими работы по ремонту энергетического оборудования.  Организация надзора за проведением электромонтажных работ при строительстве и реконструкции объектов Общества.  Составление заявок на энергоресурсы, оборудование, материалы, запасные части и инструменты.  Обеспечение повседневного управления производственной деятельностью электрохозяйства автозаправочных станций, ПЗС (нефтебаз) и систем теплоснабжения на объектах Общества.  Организация подготовки и заключение договоров с энергосбытовыми, энергоснабжающими, теплоснабжающими организациями и с организациями, выполняющими работы по ремонту и обслуживанию энергетического оборудования.  Организация работоспособности и надлежащего технического обслуживания средств учёта потребляемой электроэнергии и другого энергетического оборудования и водоснабжения.  Контроль выполнения договорных обязательств со стороны подрядных организаций.   Требования:   Опыт работы не менее 3 лет.  Стаж работы по специальности на инженерно-технических и руководящих должностях в соответствующей профилю предприятия отрасли.  Наличие допуска к работам в электроустановках: IV до и свыше 1000 В.   Условия:   Оформление по ТК РФ, полный соцпакет.  Своевременная выплата з/п.  </t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>80000</v>
+        <v>100000</v>
       </c>
       <c r="H42" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>46872889</v>
+        <v>44922061</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Аналитик данных / Начинающий аналитик данных</t>
+          <t>Инженер-энергетик</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1967,21 +1967,21 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>ФГАНУ ФЕДЕРАЛЬНЫЙ ИНСТИТУТ ЦИФРОВОЙ ТРАНСФОРМАЦИИ В СФЕРЕ ОБРАЗОВАНИЯ, ФГАНУ ФИЦТО</t>
+          <t>ГБУЗМ Городская клиническая больница № 24 ДЗМ</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/analitik-dannyh-46872889.html</t>
+          <t>https://www.superjob.ru/vakansii/inzhener-energetik-44922061.html</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Обязанности:  -  участие в организации сбора (извлечения) данных из разнородных источников (автоматизированные системы сбора данных, специализированные порталы, сайты и СУБД в области образования);  -  работа с данными (извлечение, исследование, обработка, обогащение и подготовка данных);   -  вывод и визуализация данных (формирование табличных данных, визуальных дашбордов и витрин данных);   -  настройка генерации отчетов и справок с использованием данных.   Требования:   -  уверенные знания и навыки работы с SQL, опыт работы с СУБД PostgreSQL;  -  опыт программирования на Python (стандартные библиотеки, библиотеки для анализа данных);  -  опыт работы с аналитической системой Qlik Sense;  -  не обязательными требованиями (обучим в процессе работы), но преимуществом является опыт работы с инструментами Apache NiFi, Dremio, S3, Git, а также инструментами для работы с BigData.   Условия:   -  трудоустройство по ТК РФ;  -  график работы 5/2 (с 9:00 до 18:00, в пятницу – до 16:45);  -  современный офис в шаговой доступности от метро Павелецкая;  -  конкурентная заработная плата (по результатам собеседования);  -  профессиональное обучение и развитие. </t>
+          <t xml:space="preserve"> Обязанности:   Обеспечивать бесперебойную работу, правильную эксплуатацию, ремонт и модернизацию энергетического оборудования, электрических и тепловых сетей, воздухопроводов и газопроводов.  Определять потребность производства в топливно-энергетических ресурсах, готовить необходимые обоснования технического перевооружения, развития энергохозяйства, реконструкции и модернизации систем энергоснабжения.  Контролировать соблюдение норм расхода топлива и всех видов энергии.  Осуществлять технический надзор за контрольно-измерительными, электротехническими и теплотехническими приборами, применяемыми на предприятии  </t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -1989,11 +1989,11 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>46901928</v>
+        <v>46376743</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Бизнес-аналитик розничного бизнеса (Banking)</t>
+          <t>Главный энергетик</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2003,21 +2003,21 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Банк ВТБ</t>
+          <t>Сеть гипермаркетов "Глобус"</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/biznes-analitik-roznichnogo-biznesa-46901928.html</t>
+          <t>https://www.superjob.ru/vakansii/glavnyj-energetik-46376743.html</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Обязанности:   Бизнес-планирование по основным направлениям розничного банкинга;  Аналитическая поддержка продуктовых, канальных и сегментных подразделений;  Аналитика клиентской базы (кластеризация, паттерны поведения и склонности);  Проверка гипотез и A/B тестирование;  Регулярные аналитические исследования (поиск потенциалов, точек роста, неэффективностей);    Требования:    Опыт работы в аналитике от 1 года;  Профильное образование (экономическое или техническое);  Знание методов математической статистики;  Знание SQL на уровне написания сложных запросов;  Знание языка Python (Spark, Pandas и основы ML) будут преимуществом;  Образование: Экономика, финансы, математика;    Условия:    Трудоустройство согласно Законодательству;  Конкурентная заработная плата;  Профессиональное обучение и развитие;  Добровольное медицинское страхование, льготные условия кредитования;  Корпоративная пенсионная программа, материальная помощь;  Спортивная жизнь и корпоративные мероприятия;  Возможность построить карьеру в ведущем банке России.  </t>
+          <t xml:space="preserve"> «Глобус» — международная розничная сеть гипермаркетов, представленная в Германии, Чехии и России. Компания является семейным предприятием, основанная в 1828 году в немецком городе Санкт-Вендель. Руководит компанией Томас Брух, представитель пятого поколения семьи Брух.  Первый гипермаркет «Глобус» в России открыли в 2006 году. На данный момент в составе сети 19 магазинов, расположенных в Москве, Владимире, Калуге, Климовске, Королеве, Рязани, Щелково, Ярославле, Твери, Электростали, Туле, Пушкино, Одинцово, Котельниках и Балашихе.  Наша главная ценность – сотрудники. Сегодня в команде «Глобус Россия» работают 11 000 человек. Это сотрудники гипермаркетов, логистического центра и координационного офиса компании.   Работа в «Глобус» это:    Надежный и дружный коллектив единомышленников, который ежедневно обеспечивает высокий уровень качества обслуживания покупателей. Сотрудники «Глобус» - профессионалы своего дела  Стабильность и уверенность в завтрашнем дне  Возможность развиваться профессионально и принимать непосредственное участие в развитии компании и высоких стандартов современной торговли.    Обязанности:    Организация и контроль проведения планов-предупредительных ремонтов оборудования, зданий и сооружений гипермаркета;  Организация и контроль за эксплуатацией энергосистем и инженерных коммуникаций (внутренних и наружных);  Организация и участие в межремонтных обслуживаниях, ремонте инженерного оборудования;  Технический надзор за состоянием, содержанием, ремонтом здания;  Обеспечение рационального использования материалов на выполнение ремонтных работ;  Организация и контроль эксплуатации электроустановок;  Составление отчетности, связанной с результатами деятельности инженерно-технического отдела.    Требования:    Высшее профессиональное (техническое) образование;  Опыт аналогичной работы;  IV Группы допуска по электробезопасности (до и выше 1000 В);  Удостоверение по промышленной безопасности;  Допуск по эксплуатации грузоподъемных механизмов;  Умение работать в режиме многозадачности  Готовность к обучению: желание развиваться самому и внести свой вклад в развитие компании;  Ответственное отношение к делу, внимательность;  Доброжелательность и вежливость в общении с людьми, готовность всегда прийти на помощь.    Условия:     Место работы: Гипермаркет «Глобус Митино» (м. Митино);   Гибкий график работы 5/2 (плавающие выходные);  Оформление в соответствии с ТК РФ с первого дня работы;  Работа на современном оборудовании, удобная форменная одежда;  Обучение за счет компании, возможности профессионального развития и карьерного роста;  Один из лучших соцпакетов в отрасли: льготное питание, скидка на все товары сети гипермаркетов, оформление медкнижки за счет работодателя и т.д.  </t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>115500</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -2025,11 +2025,11 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>46978335</v>
+        <v>46714312</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Инженер технической поддержки / Помощник системного администратора (стажёр)</t>
+          <t>Инженер-энергетик</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2039,33 +2039,33 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>РЕДЛАБ-И</t>
+          <t>ФКУЗ Медико-санитарная часть МВД России по г. Москве (МСЧ МВД России по г. Москве)</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/inzhener-tehnicheskoj-podderzhki-46978335.html</t>
+          <t>https://www.superjob.ru/vakansii/inzhener-energetik-46714312.html</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Обязанности    Техническая поддержка пользователей офиса, работающих под Windows: рабочие места (в т.ч. бухгалтера), резервное копирование, печать, интернет.  Участие в технической поддержке инфраструктуры компании, основанной на ОС Linux Debian: виртуальные машины/контейнеры с операционными системами под разных заказчиков, email, git, svn, x2go, веб-сайт, пакетный репозиторий (.deb) для разрабатываемых компанией продуктов.  Участие в установке, настройке и обновлении ОС и ПО, в т.ч. на территории Заказчика.  Взаимодействие с внешними пользователями: консультирование, регистрация и локализация проблем, демонстрация устранения проблем.  Взаимодействие с разработчиками: участие в постановке задач по устранению проблем, проверка устранения проблем.    Требования    Опыт администрирования ОС Windows.  Опыт диагностики, простого ремонта и обслуживания компьютеров и оргтехники.  Уверенное пользование и начальные навыки администрирования ОС Linux, желание развиваться в данной области.  Знание устройства локальных сетей на основе Ethernet, cтека TCP/IP.  Умение бережно относиться к существующей инфраструктуре.  Умение читать техническую литературу на английском языке.  Коммуникабельность, способность чётко и доходчиво излагать свои мысли при взаимодействии с пользователями.   Приветствуется   Опыт администрирования ОС Linux.  Знание скриптовых языков (bash, python).  Базовые знания С/C++.  Опыт настройки программно-управляемых L2, L3 - коммутаторов (Cisco, Huawei и т.п.): VLAN, маршрутизация.  Опыт работы с системами контроля версий (git, svn).  Опыт работы с системами отслеживания ошибок (Redmine, Jira, Trac, Bugzilla и т.п.).   Условия   Оформление с первого рабочего дня по ТК РФ.  Полная занятость, график работы 5/2.  Офис в бизнес-парке «Румянцево» (шаговая доступность от метро «Румянцево»), периодические выезды на территорию Заказчика (Москва).  Льготы, полагающиеся сотрудникам аккредитованной ИТ-компании  Возможность карьерного и профессионального роста.  </t>
+          <t xml:space="preserve">  Обязанности:   - Организационное и техническое руководство эксплуатацией и ремонтом электротехнического оборудования и электросетей.   - Обеспечение документарного сопровождение выполняемых работ- Организация эксплуатации лифтов  -Контроль выполнения персоналом работ по демонтажу и монтажу электрооборудования  - Выполнять другие необходимые обязанности по заданию руководства в соответствии с должностной инструкцией   Требования:   - Знание стандартов, правил, инструкций по эксплуатации и ремонту электротехнического оборудования и электросетей   - Умение пользоваться компьютером, офисной техникой и знание основных офисных программ   Условия:   Место работы - Клинический госпиталь, расположен по адресу: м. Войковская, г. Москва, Новая Ипатовка 3А  - Корпоративный транспорт от метро, от ж/д станции "Красный балтиец" пешком 8 мин.  Официальная заработная плата  Надбавка за стаж;  Премии, 13-я з/п, квартальные  Работа на объекте (Клинический госпиталь, м. Войковская) </t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>47000</v>
       </c>
       <c r="H45" t="n">
-        <v>75400</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>31061879</v>
+        <v>46701403</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Специалист (работа с отчетностью)</t>
+          <t>Энергетик</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2075,33 +2075,33 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>МИ ФНС России по ЦОД N2</t>
+          <t>Энергетическое Строительство</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/specialist-31061879.html</t>
+          <t>https://www.superjob.ru/vakansii/energetik-46701403.html</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Обязанности:     Контроль и загрузка в БД информации из различных источников    Формирование аналитических и статистических отчетов     Требования:    Системное и аналитическое мышление;  Умение работать с большим объемом информации.  Умение работать в режиме многозадачности.  Навыки деловой переписки, умение ясно и четко излагать свои мысли с учетом потребностей целевой аудитории.  Базовые навыки работы с офисными приложениями (MS Office Project, Word, Excel, Visio, Power Point) и браузерами, применение компьютерной и другой оргтехники,  Основы ведения делопроизводства, составление делового письма   Предпочтительно:    Продвинутые знания MS Excel, SQL    Навыки работы с MS Power Query, Python (библиотеки numpy, pandas)      Условия:   5дневная рабочая неделя, график работы пн-чт с 9 до 18, пт с 9 до 16-45, обед - 45 минут. Служебный день ненормированный (эпизодически). Отпуск составляет 30 календарных дней + 3 дня за ненормированный рабочий день+ отпуск за выслугу лет. Бесплатное обслуживание в ведомственной поликлинике. Санаторно-курортное лечение в пансионатах Сочи и Анапы. Дружный молодой коллектив. Перспективы профессионального и карьерного роста. Стабильная заработная плата. Ежеквартальное материальное стимулирование. Территориальное расположение: Походный проезд, 3, «Налоговый городок». Ближайшие станции метро: Сходненская, Тушинская, Волоколамская (10 минут общественным транспортом), а также пешая доступность от станции «Трикотажная» Рижской ЖД Полный рабочий день </t>
+          <t xml:space="preserve">  Требования:    высшее техническое образование (инженер-электрик, энергетик);  опыт работы в аналогичной должности от 3 лет;  уверенный пользователь Microsoft Office;  наличие группы по электробезопасности не ниже 4-ой;  опыт эксплуатации электротехнического оборудования;  знание требований охраны труда при эксплуатации энергетического оборудования.    Обязанности:    составление и контроль соблюдения плана производства работ;  описание и оптимизация бизнес-процессов, создание регламентов работы;  управление отношениями с субподрядными организациями, контроль выполнения работ;  взаимодействие с подразделениями в организации;  обеспечение бесперебойной работы, безопасной эксплуатации, ремонта и модернизации энергетического оборудования и электрических сетей, контроль работы инженерных систем здания.    Условия:    Оформление полностью по ТК, в штат, по трудовой книжке, как основное место работы.  Полностью официальные выплаты зарплаты (оклад+премия), два раза в месяц на банковскую карту  Заработная плата по результатам собеседования.  </t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>34123084</v>
+        <v>45941339</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Учитель информатики</t>
+          <t>Инженер-энергетик (эксплуатация)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2111,492 +2111,24 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>ГБОУ Школа №2086</t>
+          <t>Твой Дом</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>https://www.superjob.ru/vakansii/uchitel-informatiki-34123084.html</t>
+          <t>https://www.superjob.ru/vakansii/inzhener-energetik-45941339.html</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Обязанности:    Разработка рабочей программы по предмету.     Организация учебной деятельности обучающихся на уроке и во внеурочное время.     Ведение электронного журнала    Требования:   Высшее образование  стаж работы от 6 лет  опыт преподавания информатики углубленного уровня сложности в проектах ДОНМ "ИТ-класс в московской школе"; "Инженерный класс в московской школе";  результат прохождения учителем независимой диагностики в ЦНД МЦКО на уровень не ниже высокого  результативность подготовки к ОГЭ, ЕГЭ   Программирование: Перволого/Логомиры, Scratch, Кумир, Паскаль/Дельфи, Alice/Greenfoot/Java, C/C++, Python  САПР: Компас  Веб-дизайн и разработка: HTML5, CSS3, JavaScript, JQuery, PHP, Adobe Photoshop, Dreamweaver, Flash, AJAX  СУБД: SQL (Oracle APEX), MySQL  Администрирование: Windows, Linux, Cisco      Условия:  Школа на протяжении ряда лет входит в 50 лучших школ по итогам рейтинга вклада ОО в качественное образование московских школьников; по итогам 2021-2022 уч.года школа удостоена Гранта Мэра 2 степени за достижение высоких результатов образовательной деятельности.  Школа участвует в проектах ДОНМ "ИТ-класс в московской школе" (направление - программирование); "Инженерный класс в московской школе". </t>
+          <t xml:space="preserve">  ТВОЙ ДОМ - не имеющая аналогов по товарному ассортименту, сеть гипермаркетов, входящая в состав крупнейшего российского холдинга CROCUS GROUP. По истине уникальная торговая площадка, сочетающая 7 гипермаркетов под одной крышей! Тысячи брендов. Более 300 тысяч наименований товаров различных категорий: товары для дома, ремонта, дизайна, мебельный салон, оранжерея, гастроном и многое другое. Здесь каждый соискатель найдет для себя сферу для профессионального развития и личностного роста. Стань частью амбициозной команды ТВОЙ ДОМ!    Обязанности:    организация работ по обеспечению работоспособности электрооборудования;  организация ремонтных работ при обнаружении неполадок в работе электрооборудования;  обеспечение электробезопасности сотрудников предприятия;  контролирование работы подчиненного линейного персонала на объекте;  диагностика, ремонт и настройка светодиодного электрооборудования освещения комплекса.   Требования:   высшее профильное образование;  опыт работы на аналогичной должности;  знание инженерных систем;  Условия:  оформление по ТК РФ;  график работы 5/2 9-18;  оплата больничных и отпусков.  место работы: МКАД, 24-й км, м. Домодедовская   Работа в нашей команде - это возможность реализовать свои идеи, получить бесценный опыт и расти вместе с компанией </t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>86000</v>
       </c>
       <c r="H47" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>34424249</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>DevOps Engineer</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>SuperJob</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/devops-engineer-34424249.html</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> SuperJob — это инновационная IT-компания, которая помогает соискателям найти работу, а работодателям — приобрести ценного сотрудника.  Ежемесячно нашим сервисом пользуются миллионы соискателей и десятки тысяч работодателей, среди которых РЖД, Мегафон, МТС, Леруа Мерлен, Почта России, Сбербанк, Альфа-Банк, Ригла и многие другие. Мы активно развиваем нашу платформу и делаем ее лучше, подтверждая миссию «Работа должна доставлять удовольствие!»   Мы ожидаем от кандидата опыт:    Администрирования Linux.  Настройки и эксплуатации CI/CD.  Программирования (скрипты Bash/PHP/Python/Go).  Настройки и эксплуатации web-проектов.  Использования систем мониторинга.    Чем предстоит заниматься:    Управлять мониторингом zabbix, grafana.  Создавать и развивать собственные инструменты мониторинга и профайлинга для внутренних сервисов (php, nodejs) и для используемого стороннего ПО.  Реагировать на инциденты, не теряя присутствия духа.  Поддерживать актуальный план восстановления в случае сбоев.  Проводить нагрузочное тестирование новых сервисов, новых версий и новых конфигураций для mariadb и других серверов.  Находить узкие места в архитектуре проекта и приложений.  Рулить конфигурацией сервисов nginx, mariadb, clickhouse, apache, rabbitmq и других.  Писать плейбуки и роли для ansible для конфигурации и деплоя.  Контейнеризировать новые сервисы и поддерживать старые.  Поддерживать стороннее ПО (sentry, testrail, confluence, jira, bitbucket, teamcity).  Рулить процессом continuous integration и deployment.    Будет плюсом опыт:    Администрирования систем виртуализации.  Администрирования баз данных SQL, NoSQL.  Администрирования высоконагруженного web-проекта.   Мы используем в работе свой дата-центр, пару сотен серверов, CentOs/Virtuozzo, Git, Nginx, Apache, NodeJS, Bash/Sh, PHP, Python, Rust, Go, MariaDB/MySql, PostgreSQL, Redis, Sphinx, RabbitMQ, Memcache, ClickHouse, ELK, Graphite/Grafana, Zabbix, TeamCity, Jenkins, Docker, Ansible, Nexus, Vault, Atlassian Jira/Confluence/BitBucket.   Своему будущему коллеге мы предлагаем:    Работу в одном из самых быстрорастущих рынков - HRTech.   Высокую инженерную культуру.   Непрерывное обучение и профессиональное развитие внутри компании.   Возможность стать частью сплоченной команды, любящей свое дело.   Регулярную обратную связь от наставников и руководителей.   Официальную заработную плату.   ДМС после прохождения испытательного срока.   Современный офис в 10 минутах пешей прогулки от станций метро Пушкинская/Маяковская/Чеховская/Новослободская.   Спортивный уголок.   Комфортную зону отдыха.   Кофе-поинты с вкуснейшим кофе и вендинговым аппаратом.   Оборудованное просторное место для питания.   Оплату проезда общественным транспортом.   </t>
-        </is>
-      </c>
-      <c r="G48" t="n">
-        <v>0</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>43137935</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Системный администратор, IT-специалист</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>ФГБУ "Научно-исследовательский центр космической гидрометеорологии "Планета"</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/sistemnyj-administrator-43137935.html</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Обязанности:  •  настройка и эксплуатация межсетевых экранов, маршрутизаторов, систем мониторинга за трафиком и безопасностью;   •  поиск и устранение неисправностей сети, уязвимостей сети;  •  настройка мониторинга работоспособности оборудования, каналов связи (zabbix);  •  работа с системами виртуализации (hyper-v; vmware; контейнеры docker и др.);   • настройка ОС Linux (CentOS, openSUSE и др.), Asta linux, Windows (7,10, server 2012 – 2019);    • автоматизация рутиных задачь;    • участие в эксплуатации и развитии ИТ-инфраструктуры организации;      •  разработка документации (схемы, руководства по эксплуатации, описания) в рамках круга обязанностей;    • антивирусная защита;    •  участие в монтажных работах по СКС (редко);   •  участие в установке и развертывании серверного оборудования, систем хранения данных, сетевого оборудования (редко);  •  администрирование видеоконференцоборудования (работа по графику).        Требования:     образование высшее (допускается обучение в магистратуре, вечернее отделение);    работа с ОС Linux (CentOS, openSUSE и др.), Asta linux, Windows (7,10, server 2012 – 2019) на уровне администратора;      Обязательно знание:    протоколы передачи данных по ЛВС;     характеристики и основы эксплуатации сетевого оборудования (коммутаторы, маршрутизаторы, межсетевые экраны);    устройство и принципы работы ЭВМ и периферийного оборудования (принтеры, МФУ, мониторы);    устройство и работа с серверного оборудования;      написание скриптов, умение программировать на языке  Python приветствуется;    читать техническую документацию на английском языке;    наличие опыта работы системным администратором является преимуществом;    Наличие сертификатов повышения квалификации в сфере IT является преимуществом.     Условия:    Работа в центре Москвы (м. Краснопресненская).   график работы 5/2 с 9 до 18 часов;  Постоянная работа;  Дружная профессиональная команда;  Оформление по ТК РФ;  Интересные КОСМИЧЕСКИЕ проекты;  Возможности карьерного роста (Компания постоянно развивается и растёт).  Уровень зарплаты обсуждается с успешным кандидатом.    Уважаемые соискатели,  просьба указывать ожидаемый уровень З/П на руки в сопроводительном письме!  </t>
-        </is>
-      </c>
-      <c r="G49" t="n">
-        <v>0</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>43148990</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Инженер-радиоэлектронщик 1 категории</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Радиофизика</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/inzhener-radioelektronschik-1-kategorii-43148990.html</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Обязанности:     - участие в проектировании устройств по ТЗ - написание программ для микроконтроллеров различных производителей (Atmel, STM32 и др.) - написание прикладных программ для ПК - разработка и согласование технических заданий и технических условий.     Требования:    - высшее (техническое) образование - знание С++, Python, Java - опыт работы с контроллерами Atmel, Cortex - приветствуются знания схемотехники, оптоэлектроники, умение паять и т.п.       Условия:   - работникам ПАО "Радиофизика" предоставляется право на отсрочку от призыва на военную службу по мобилизации;  - стабильная, официальная заработная плата;  - периодическая индексация заработной платы;  - периодический медицинский осмотр;  - соц. пакет: дополнительное медицинское обслуживание;  - ст. м. Планерная, ул. Героев Панфиловцев, д. 10 (шаговая доступность от станции метро). </t>
-        </is>
-      </c>
-      <c r="G50" t="n">
-        <v>100000</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>45760672</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Системный администратор</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>ТБ ПРОЕКТ</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/sistemnyj-administrator-45760672.html</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Обязанности:    Поддержание рабочего состояния рабочих станций  Поддержка пользователей (включая удаленную)  Участие в развитии внутренней инфраструктуры, её техническое сопровождение    Требования:    Понимание основ сети (TCP/IP, DNS, VPN, VLAN, DHCP)   Навыки работы с Windows Server – TS, AD, GPO, WSUS, Hyper-V   Минимальный опыт администрирования БД MSSQL   Базовые навыки администрирования Windows и *nix   Настройка базового бухгалтерского ПО – CryptoPro, контур, такском, 1C    Желательно:   Zabbix   FreePBX/Asterisk   Cisco ASA, Juniper EX   *nix: bash, exim4, dovecot, nginx, php-fpm, gunicorn   Знание python на минимальном уровне     С чем предстоит работать:    Кластер на базе Hyper-V  MS инфраструктура включая SCCM, DPM, MSSQL.  Сетевое оборудование Cisco ASA, Juniper EX, Ubiquity   IP телефония на базе FreePBX   Более 100 пользователей   Несколько офисов на территории г. Москва и ближайшее Подмосковье.     98% времени работа в офисе по адресу Амундсена, 9, но редкие выезды в другие офисы будут      Условия:    формление по ТК РФ;   официальная з/п   график работы 5/2;   шаговая доступность от метро Свиблово (7 мин).   полный рабочий день (с 9.00 до 18.00)   на территории работодателя  </t>
-        </is>
-      </c>
-      <c r="G51" t="n">
-        <v>0</v>
-      </c>
-      <c r="H51" t="n">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>46296647</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Учитель информатики</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Школа №2116</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/uchitel-informatiki-46296647.html</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Обязанности:    Качественное ведение уроков информатики (1,5 ставки - классы обсуждаются)   Подготовка к экзаменам и олимпиадам, городским конференциям и конкурсам,   Ведение внеурочной деятельности, дополнительного образования   Требования:   Высшее профильное образование  Диагностика МЦКО (высокий/экспертный уровень по информатике)   Опыт работы учителем информатики (подготовка к ОГЭ/ЕГЭ, олимпиадам и конференциям)   Владение ПК   Справка о несудимости (обязательно!)   Медицинская книжка и пр. документы, предусмотренные ТК РФ для пед.работников   Условия:   Стабильная заработная плата и стимулирующие выплаты  Социальный пакет (оплата отпусков, листков нетрудоспособности, повышение квалификации и пр.)   Сотрудник требуется с 1 сентября 2023 г.  В сопроводительном письме к отклику просьба указать уровень диагностики МЦКО </t>
-        </is>
-      </c>
-      <c r="G52" t="n">
-        <v>100000</v>
-      </c>
-      <c r="H52" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>46276186</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Ведущий системный администратор</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>СМ-Клиника</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/veduschij-sistemnyj-administrator-46276186.html</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> МНОГОПРОФИЛЬНЫЙ МЕДИЦИНСКИЙ ХОЛДИНГ «СМ-КЛИНИКА» - это одна из крупнейших сетей многопрофильных медицинских центров для взрослых и детей, ведущая историю своего существования с 2002 года.  ОБЯЗАННОСТИ:   Администрирование, настройка и сопровождение виртуальных серверов на базе Linux и Windows  Администрирование, настройка и сопровождение виртуальной инфраструктуры VMWare  Администрирование, настройка и сопровождение СУБД, MS SQL, MySQL, PostgreSQL, no SQL  Администрирование, настройка и сопровождение физических серверов и СХД  Настройка и поддержка окружения для команды разработчиков (сервисы на Linux)  Автоматизация процессов обслуживания серверов  Резервное копирование СУБД и серверов (Veeam)  Сопровождение почтового сервера (Zimbra)  Сопровождение системы мониторинга Zabbix  Сопровождение оборудования в ЦОДа  Мониторинг производительности и оптимизация работы серверов и сервисов  Проведение регламентных работ на оборудовании и платформы виртуализации  Документирование виртуальной и серверной инфраструктуры и вносимых изменений  3й уровень поддержки пользователей   ТРЕБОВАНИЯ:   Высшее техническое образование  Опыт работы системным администратором не менее 6 лет  Глубокие знание ОС Linux Centos, Fedora (понимание работы iptables)  Глубокие знания серверных ОС Windows и базовых сервисов - AD, DHCP, DNS, RDS, IIS, WSUS и т.д.  Знание (установка, конфигурирование, обслуживание) Apache, Nginx, Ha-proxy, Keepalived, RabbitMQ, Squid  Знание сетевых протоколов (понимание маршрутизации ipv4)  Опыт работы с SCM-системами Ansible/Chef/Puppet  Опыт работы с продуктами Atlassian (Jira,Confluence)  Опыт эксплуатации сервисов высокой доступности  Опыт работы с СХД (NetApp/VSAN/VxFlex) уровня предприятия - внедрение и сопровождение  Опыт внедрения и поддержки платформ виртуализации  VMWARE в промышленной среде  Опыт настройки систем резервного копирования  Опыт написания скриптов на Bash, Powershell, Python  УСЛОВИЯ:  График работы 5/2 (09.00-18.00)  Территориально ул. Аргуновская 3 к.2 м. ВДНХ  Дополнительное обучение в корпоративном учебном центре (повышение квалификации, сертификационное обучение, обучение управленческим навыкам)  Возможность развития в рамках программы «Кадровый резерв»  Льготное медицинское обслуживание для сотрудников в клиниках Холдинга (включая стоматологию, косметологию) и скидки для членов семьи  Скидки для сотрудников в аптеках сети Холдинга  Корпоративное питание в кафе клиник  Специальные тарифы на отдых в загородном Парк-Отеле  Бесплатные спортивные секции для сотрудников (футбол, волейбол, танцы, йога, вокал, киберспорт)  Корпоративные программы и специальные предложения от партнеров Холдинга  </t>
-        </is>
-      </c>
-      <c r="G53" t="n">
-        <v>160000</v>
-      </c>
-      <c r="H53" t="n">
-        <v>180000</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>46215550</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Системный инженер SOC (ELK)</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>РТ-Информационная безопасность</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/sistemnyj-inzhener-soc-46215550.html</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Обязанности:    Администрирование и развитие системы мониторинга центра на основе ELK стека;  Интеграция средств защиты информации различных вендоров с ELK, работа с плагинами, dashboard, визуализацией, агрегацией, конфигураций pipeline;  Обеспечение отказоустойчивости и непрерывной работы ELK стека и связанных сервисов.  Разработка предложений по интеграции новых сервисов и оптимизации работы существующих;  Внешняя и внутренняя поддержка ELK стека;  Разработка коннекторов к СЗИ.   Обязательные требования:   Профильное образование или профессиональная переподготовка;  Опыт администрирования кластера elasticsearch, введения в строй отказоустойчивого кластера, бекапирования и восстановления;  Опыт администрирования и работа с ОС Linux, докерами и оркестраторами;  Опыт работы с СУБД, системами мониторинга;  Знание практических принципов информационной безопасности;  Опыт написания скриптов автоматизации на Python, Bash для задач по администрированию ИТ-инфраструктуры.   Будет преимуществом:   Опыт работы с различными СЗИ;  Опыт построения CI/CD инфраструктуры;  Опыт администрирования ИТ-инфраструктуры.    Условия:    Оформление по ТК РФ  Полная занятость  Возможность профессионального и карьерного роста  Заработная плата по результатам собеседования  Корпоративный транспорт до метро Южная  </t>
-        </is>
-      </c>
-      <c r="G54" t="n">
-        <v>160000</v>
-      </c>
-      <c r="H54" t="n">
-        <v>280000</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>46708119</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Преподаватель спец. дисциплин (сетевой и системный администратор)</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>ГОУ СПО Колледж связи</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/prepodavatel-spec-46708119.html</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Обязанности:    преподавание междисциплинарных курсов в группах СПО:     ОП.03 Информационные  технологии    ДУД.06 Программирование на  языке сценариев командной оболочки    ОП.14 Настройка, обновление и конфигурация операционных систем      Требования:     образование, знания,   умения - в соответствии с Профстандартом.     владение навыками работы   в специализированных программах, а также: Microsoft Excel, Microsoft   Outlook, Microsoft PowerPoint, Microsoft Word, Интернет, электронная   почта.     История ОС, архитектура.   Диспетчеризация, планирование и взаимодействие процессов ОС, работы с   памятью, файловые системы, принципы организации. Установка, настройка и   работы в Windows, Linux, Astra Linux. Администрирование ОС и управление   безопасностью     Сертификаты Cisco/Huawei либо иных   сетевых вендоров. Плюсом будут сертификаты Microsoft и Python, Astra   Linux (или иных Linux дистрибутивов)     Знание модели OSI/   Принцип работы протоколов TCP и UDP     Знание сетевых   протоколов. FTP, SMTP, POP, IMAP, DHCP, IPv6 адресации. Протоколы   удалённого доступа (SSH, Telnet). Принцип работы сети на физическом   уровне. Принцип работы технологий IEEE 802.11 (WiFi) Понимание принципа   роботы локальных сетей.Ipv6 адресация, SLAAC + DHCPv6. Технологии WPAN,   WLAN, WMAN, WWAN. Технологии беспроводной связи BLE, BR/EDR, WiMAX.     Медицинская книжка,   медицинское освидетельствование психиатр/нарколог, справка об отсутствии   судимости        Условия:        Работа на территории работодателя        Полный социальный пакет    Отпуск в летнее время     </t>
-        </is>
-      </c>
-      <c r="G55" t="n">
-        <v>80000</v>
-      </c>
-      <c r="H55" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>46883126</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Инженер сопровождения программного обеспечения</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Викей</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/inzhener-soprovozhdeniya-programmnogo-obespecheniya-46883126.html</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Обязанности: &lt;ol&gt; Участие в новых проектах компании  Взаимодействие с разработчиками программного обеспечения по задачам, требующим доработки или исправления ПО  Проведение экспертиз для поисков решений, направленных на устранение потенциальных проблем в программном обеспечении  Поддержка установленных систем  Проведение тестирования программного обеспечения  Подбор и сборка оборудования  Участие в пусконаладке разработанных систем  Разработка верхнеуровневой документации  Проведение внутренних презентаций/обучения разработанных систем &lt;/ol&gt; Требования: &lt;ol&gt;  Работа с ОС семейства Unix/Windows    Опыт работы и администрирования серверного оборудования    Опыт работы с embedded системами и одноплатными компьютерами    Опыт сборки различных устройств и их компонентов    Опыт написания скриптов (bash / python / Perl …)    Знакомство с принципами работы БД (sql, nosql) и основами языка sql и понимание его семантики    Опыт владения системами контейнеризации (Docker, Docker compose) и виртуализации    Понимание принципов разработки ПО, архитектуры ПО и сетей, методик и видов тестирования ПО и оборудования    Опыт в тестировании ПО и оборудования     Опыт в диагностике и устранении ошибок в работе компьютерного оборудования (как в части ПО, так и в “железной” части)    Опыт работы с системами контроля версий GitHub / git lab / bit bucket     Владение английском языком (минимум: понимание документации, возможность проводить презентации по заранее изученному тексту)    Готовность работы в стартапах внутри компании    Опыт работы и написания технической документации, функциональных требований, ведение инвентаризационных документов отдела, методик приемно-сдаточных работ    Готовность к командировкам    Инициативность    Коммуникабельность    Аналитический склад ума    Будет плюсом умение работы с 3D моделями для печати на 3D принтере  &lt;/ol&gt;  Условия:     работа в стабильной компании, работающей по международным стандартам;    оформление согласно ТК РФ (ежегодный оплачиваемый отпуск, оплачиваемый больничный лист);    пятидневная рабочая неделя,  работа в офисе, строго не удаленно;     работа в молодом, дружном коллективе;    уютный, комфортный офис в 7 минутах от м. Динамо.   </t>
-        </is>
-      </c>
-      <c r="G56" t="n">
-        <v>90000</v>
-      </c>
-      <c r="H56" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>45695529</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Программист Linux</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Фактор-ТС</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/programmist-linux-45695529.html</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Требования:   Знание TCP/IP;  Умение работать с системами контроля версий;  Желательно: опыт написания переносимого и безопасного кода;  Желательно: опыт написания кода ядра;  Желательно: понимание архитектуры современных ОС.  Хорошее знание C;  Хороший опыт работы в Unix системах, знание основных утилит командной строки, средств отладки.  Представление о системах контроля версий git (или svn).  Опыт отладки в gdb.  Представление об утилите make и мейкфайлах.   Желательные знания:    Знание C++, lua, Go lang, qt.  Знание хотя бы одного из скриптовых языков: perl, python, lua.  Представление об autoconf, automake.  Представление об утилите и/или библиотеке openssl.  Базовые представления о криптографии: симметричные и асимметричные ключи, сертификаты, шифрование, электронная подпись.  Большим плюсом будет наличие представления о формате ASN.1.   Условия:    Зарплата обсуждается в зависимости от опыта работы, уровня квалификации и соответствия требованиям вакансии;  Возможность профессионального и карьерного роста;   Оформление по ТК РФ (трудовой договор, трудовая книжка);   Расположение офиса: между м. ул. 1905 г. и м. Беговая (с 8-00 до 20-30 автобус компании по расписанию возит сотрудников к / от метро).    </t>
-        </is>
-      </c>
-      <c r="G57" t="n">
-        <v>100000</v>
-      </c>
-      <c r="H57" t="n">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>46932043</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Преподаватель по направлению Информационные системы и Программирование</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>ГБПОУ Колледж Москва</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/prepodavatel-po-napravleniyu-informacionnye-sistemy-i-programmirovanie-46932043.html</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Обязанности:    Проведение занятий по учебным предметам, курсам, дисциплинам (модулям) образовательной программы в соответствии с расписанием учебных занятий.   Разработка и обновление рабочих программ учебных предметов, курсов, дисциплин (модулей) и т.д.    Ведение документации   Требования:   Знание/понимание алгоритмов и языков программирования (C#, C++, JS, PHP, Python — уровень выше среднего).  Знание методов программирования    Условия:    Официальное трудоустройство согласно ТК РФ;   36 часовая рабочая неделя;   Адрес места работы: г. Москва, ул. Пресненский Вал, д. 15, стр. 1 (ближайшая станция метро Улица 1905 года).  </t>
-        </is>
-      </c>
-      <c r="G58" t="n">
-        <v>0</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>46935497</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Аналитик данных</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>АВАНГАРД</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/analitik-dannyh-46935497.html</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Занимается оптово-розничной продажей электроинструментов на маркетплейсах  Почему Ты должен выбрать именно нас:   Современный подход к работе   Любая поддержка для увеличения вашей продуктивности, комфорта, оптимизации ваших действий за счет компании   Своевременные выплаты заработной платы два раза в месяц  Обязанности:  Сбор, хранение информации и бизнес-показателей  Подготовка и обработка полученных сведений (сортировка, группировка, сведение, запросы к базам данных, создание гугл-таблиц, написание сложных формул, автоматизация отчетов и расчетов)  Анализ полученных сведений: нахождение закономерностей, классический анализ табличных данных, критический анализ идей и информации  Анализ и контроль динамики позиций на маркетплейсах, анализ рекламных расходов, анализ финансовых показтелей (маржиналонсти, оборачиваемости, сведение данных из разных источников), анализ продаж и их динамики, прогнозирование трендов продаж, анализ рынков  Составление гипотез, трактовка аномалий, проектирование решений, контроль за основными показателями,  Визуализация данных, доступное объяснение полученных данных  Проведение когортного анализа и А/В-тестирования карточек товара, баннеров и прочее    Требования: Hard skill  Знание инструментов SQL, Python;  Отличное знание MS Office, в частности Excel  Знания форматов обмена данными, таких как CSV, XML, JSON  Знания методов парсинга данных через API  Умение работать с большим объемом данных  Владение различными методами визуализации (дашборды, графики и прочее)  Знания методов анализа и статистики  Умение работать с Google Sheets, знание принципов и понимание работы макросов, а также умение их писать   Личные качества (Soft skill):   Концентрация  Усидчивость  Структурная логика  Аналитический склад ума  Способность выявлять проблемы и решать их  Целеустремленность  Умение аргументированно высказывать свое мнение  Гибкость мышления  Навыки планирования  Желание обучаться     Условия:   Работа в офисе с 10:00 до 19:00 полной занятостью (5/2)  Испытательный срок 1 месяц  Заработная плата от 100 000 - 150 000 руб  Официальное трудоустройство после 3-х месяцев работы  Работа с интересными товарами в молодом дружном коллективе, возможность получения новых знаний и навыков!  Теплая и дружная атмосфера  Возможность профессионального роста и реализации идей  Своевременные выплаты заработной платы  Комфортный офис, в котором всегда есть: чай, фрукты, снэки  Если вы изучили вакансию и готовы присоединиться к нашей команде, отправляйте свой отклик, и в сопроводительном письме напишите проверочную фразу "Контрольная точка"  </t>
-        </is>
-      </c>
-      <c r="G59" t="n">
-        <v>100000</v>
-      </c>
-      <c r="H59" t="n">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>46960844</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Главный разработчик</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Москва</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Группа компаний МАСКОМ/ООО "ЦБИ "МАСКОМ"</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>https://www.superjob.ru/vakansii/glavnyj-razrabotchik-46960844.html</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   Обязанности:    организация процесса разработки модулей к существующему ПО с помощью подчиненных, CodeReview   развитие существующего ПО   обсуждение пожеланий по доработке ПО с заказчиком   разработка документации для программистов (по сути, не ГОСТ)   Требования:    опыт разработки от 5 лет    разработки в команде с программистами в подчинении и самостоятельно   наличие завершенных проектов с backend на Python.   умение самостоятельно развернуть проект под Linux.  Git, GitHub, Confluence, Jira     Языки: Python, JavaScript, желательно Dart  Фреймворки: желательно Flutter   Базы данных: PostgreSQL, SQLite   Условия:   Зарплата полностью официально.   Трудоустройство в компании аккредитованной в Мин. цифре.   Бронь.   Гибкий график.   Возможность работать удаленно.   Возможны командировки.  Офис м. Октябрьское поле, 5 минут пешком.     </t>
-        </is>
-      </c>
-      <c r="G60" t="n">
-        <v>200000</v>
-      </c>
-      <c r="H60" t="n">
-        <v>0</v>
+        <v>86000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>